<commit_message>
updated teamreport and changed unit32test-> unit_test
</commit_message>
<xml_diff>
--- a/TeamXXReport.xlsx
+++ b/TeamXXReport.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StevensUser\Documents\Junior Year\Spring 2019\Agile Methods for Software Dev\Week 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chloequinto/Documents/SSW_555_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9165C424-64B8-FA48-B2F7-C2DA919A183A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="460" windowWidth="27300" windowHeight="15480" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="1480" yWindow="460" windowWidth="27300" windowHeight="15480" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="287">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -908,12 +909,36 @@
   </si>
   <si>
     <t>https://github.com/chloequinto/SSW_555_Project</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>us32.py</t>
+  </si>
+  <si>
+    <t>checkMultipleBirths</t>
+  </si>
+  <si>
+    <t>24-86</t>
+  </si>
+  <si>
+    <t>unit_test.py</t>
+  </si>
+  <si>
+    <t>test_multipleBirths</t>
+  </si>
+  <si>
+    <t>13-21</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -1209,7 +1234,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1280,7 +1305,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2260,22 +2285,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="150" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.69140625" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="5" width="20.4609375" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2292,7 +2317,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>200</v>
       </c>
@@ -2309,7 +2334,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>205</v>
       </c>
@@ -2326,7 +2351,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>215</v>
       </c>
@@ -2343,7 +2368,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="20" t="s">
         <v>240</v>
       </c>
@@ -2360,7 +2385,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" s="20" t="s">
         <v>243</v>
       </c>
@@ -2377,7 +2402,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="D9" s="4" t="s">
         <v>35</v>
       </c>
@@ -2391,12 +2416,12 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D4" r:id="rId2"/>
-    <hyperlink ref="D5" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4" display="mwisnews@stevens.edu"/>
-    <hyperlink ref="D7" r:id="rId5"/>
-    <hyperlink ref="D6" r:id="rId6"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E5" r:id="rId4" display="mwisnews@stevens.edu" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D6" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2404,23 +2429,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.15234375" customWidth="1"/>
-    <col min="2" max="2" width="7.69140625" customWidth="1"/>
-    <col min="3" max="3" width="26.15234375" customWidth="1"/>
-    <col min="4" max="4" width="6.69140625" customWidth="1"/>
-    <col min="5" max="5" width="7.69140625" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2437,7 +2462,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2454,7 +2479,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2471,7 +2496,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2488,7 +2513,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2505,7 +2530,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2522,7 +2547,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2539,7 +2564,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2556,7 +2581,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2573,7 +2598,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2590,7 +2615,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2604,10 +2629,10 @@
         <v>200</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2621,7 +2646,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2635,7 +2660,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2649,7 +2674,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2663,7 +2688,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2677,7 +2702,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2691,7 +2716,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2705,7 +2730,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2719,7 +2744,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>2</v>
       </c>
@@ -2733,7 +2758,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>2</v>
       </c>
@@ -2747,7 +2772,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>3</v>
       </c>
@@ -2761,7 +2786,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>3</v>
       </c>
@@ -2775,7 +2800,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>3</v>
       </c>
@@ -2789,7 +2814,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>3</v>
       </c>
@@ -2803,7 +2828,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>3</v>
       </c>
@@ -2817,7 +2842,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>3</v>
       </c>
@@ -2831,7 +2856,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>3</v>
       </c>
@@ -2845,7 +2870,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>3</v>
       </c>
@@ -2859,7 +2884,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2873,7 +2898,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2887,7 +2912,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>4</v>
       </c>
@@ -2901,7 +2926,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>4</v>
       </c>
@@ -2915,7 +2940,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>4</v>
       </c>
@@ -2929,7 +2954,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>4</v>
       </c>
@@ -2943,7 +2968,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>4</v>
       </c>
@@ -2957,7 +2982,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>4</v>
       </c>
@@ -2971,7 +2996,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>4</v>
       </c>
@@ -2985,7 +3010,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>4</v>
       </c>
@@ -2999,7 +3024,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>4</v>
       </c>
@@ -3013,7 +3038,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>4</v>
       </c>
@@ -3035,54 +3060,54 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView topLeftCell="A8" zoomScale="150" workbookViewId="0">
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.84375" style="7"/>
-    <col min="2" max="2" width="9.4609375" customWidth="1"/>
-    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3046875" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>167</v>
       </c>
@@ -3105,7 +3130,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>168</v>
       </c>
@@ -3121,7 +3146,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>169</v>
       </c>
@@ -3146,7 +3171,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
         <v>170</v>
       </c>
@@ -3171,7 +3196,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
         <v>171</v>
       </c>
@@ -3196,7 +3221,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>172</v>
       </c>
@@ -3229,24 +3254,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.53515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.69140625" customWidth="1"/>
-    <col min="3" max="3" width="12.4609375" customWidth="1"/>
-    <col min="4" max="4" width="7.15234375" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="17.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3266,7 +3291,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>264</v>
       </c>
@@ -3277,7 +3302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>265</v>
       </c>
@@ -3286,17 +3311,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>268</v>
       </c>
@@ -3310,34 +3335,35 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.84375" customWidth="1"/>
-    <col min="2" max="2" width="35.84375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.3046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="37.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="9.15234375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.4609375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.3046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.4609375" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.15234375" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.1640625" style="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.84375" style="17" customWidth="1"/>
-    <col min="15" max="15" width="10.15234375" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.4609375" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.15234375" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.83203125" style="17" customWidth="1"/>
+    <col min="15" max="15" width="17" style="17" customWidth="1"/>
+    <col min="16" max="16" width="21.83203125" style="17" customWidth="1"/>
+    <col min="17" max="17" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3384,7 +3410,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>113</v>
       </c>
@@ -3431,7 +3457,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="20" t="s">
         <v>232</v>
       </c>
@@ -3445,7 +3471,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="20" t="s">
         <v>233</v>
       </c>
@@ -3457,7 +3483,7 @@
       </c>
       <c r="D4" s="20"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="20" t="s">
         <v>234</v>
       </c>
@@ -3469,7 +3495,7 @@
       </c>
       <c r="D5" s="20"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="20" t="s">
         <v>235</v>
       </c>
@@ -3481,7 +3507,7 @@
       </c>
       <c r="D6" s="20"/>
     </row>
-    <row r="7" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="20" t="s">
         <v>236</v>
       </c>
@@ -3493,14 +3519,14 @@
       </c>
       <c r="D7" s="20"/>
     </row>
-    <row r="8" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="20"/>
       <c r="B8" s="22"/>
       <c r="C8" s="20"/>
       <c r="D8" s="20"/>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
         <v>218</v>
       </c>
@@ -3538,7 +3564,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="20" t="s">
         <v>253</v>
       </c>
@@ -3552,7 +3578,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="20" t="s">
         <v>254</v>
       </c>
@@ -3563,7 +3589,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="20" t="s">
         <v>255</v>
       </c>
@@ -3574,12 +3600,12 @@
         <v>205</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
       <c r="B13" s="22"/>
       <c r="C13" s="20"/>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>115</v>
       </c>
@@ -3597,7 +3623,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -3613,7 +3639,7 @@
       <c r="I15" s="7"/>
       <c r="K15" s="18"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>156</v>
       </c>
@@ -3626,7 +3652,7 @@
       <c r="I16" s="7"/>
       <c r="K16" s="18"/>
     </row>
-    <row r="17" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>157</v>
       </c>
@@ -3639,13 +3665,13 @@
       <c r="I17" s="7"/>
       <c r="K17" s="18"/>
     </row>
-    <row r="18" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="22"/>
       <c r="C18" s="20"/>
       <c r="I18" s="7"/>
       <c r="K18" s="18"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
         <v>116</v>
       </c>
@@ -3663,7 +3689,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="20" t="s">
         <v>250</v>
       </c>
@@ -3679,7 +3705,7 @@
       <c r="I20" s="7"/>
       <c r="K20" s="18"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="20" t="s">
         <v>251</v>
       </c>
@@ -3692,7 +3718,7 @@
       <c r="I21" s="7"/>
       <c r="K21" s="18"/>
     </row>
-    <row r="22" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="20" t="s">
         <v>252</v>
       </c>
@@ -3705,13 +3731,13 @@
       <c r="I22" s="7"/>
       <c r="K22" s="18"/>
     </row>
-    <row r="23" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="22"/>
       <c r="C23" s="20"/>
       <c r="I23" s="7"/>
       <c r="K23" s="18"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
         <v>117</v>
       </c>
@@ -3729,7 +3755,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="20" t="s">
         <v>158</v>
       </c>
@@ -3745,7 +3771,7 @@
       <c r="I25" s="7"/>
       <c r="K25" s="18"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="20" t="s">
         <v>159</v>
       </c>
@@ -3758,7 +3784,7 @@
       <c r="I26" s="7"/>
       <c r="K26" s="18"/>
     </row>
-    <row r="27" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="20" t="s">
         <v>160</v>
       </c>
@@ -3771,13 +3797,13 @@
       <c r="I27" s="7"/>
       <c r="K27" s="18"/>
     </row>
-    <row r="28" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="22"/>
       <c r="C28" s="20"/>
       <c r="I28" s="7"/>
       <c r="K28" s="18"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
         <v>118</v>
       </c>
@@ -3795,7 +3821,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A30" s="20" t="s">
         <v>223</v>
       </c>
@@ -3811,7 +3837,7 @@
       <c r="I30" s="7"/>
       <c r="K30" s="18"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A31" s="20" t="s">
         <v>224</v>
       </c>
@@ -3824,7 +3850,7 @@
       <c r="I31" s="7"/>
       <c r="K31" s="18"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A32" s="20" t="s">
         <v>225</v>
       </c>
@@ -3837,14 +3863,14 @@
       <c r="I32" s="7"/>
       <c r="K32" s="18"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A33" s="20"/>
       <c r="B33" s="20"/>
       <c r="C33" s="20"/>
       <c r="I33" s="7"/>
       <c r="K33" s="18"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
         <v>219</v>
       </c>
@@ -3859,7 +3885,7 @@
       </c>
       <c r="I34" s="7"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A35" s="20" t="s">
         <v>256</v>
       </c>
@@ -3874,7 +3900,7 @@
       </c>
       <c r="I35" s="7"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A36" s="20" t="s">
         <v>257</v>
       </c>
@@ -3886,7 +3912,7 @@
       </c>
       <c r="I36" s="7"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A37" s="20" t="s">
         <v>258</v>
       </c>
@@ -3898,13 +3924,13 @@
       </c>
       <c r="I37" s="7"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A38" s="20"/>
       <c r="B38" s="20"/>
       <c r="C38" s="20"/>
       <c r="I38" s="7"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
         <v>144</v>
       </c>
@@ -3915,10 +3941,43 @@
         <v>200</v>
       </c>
       <c r="D39" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+        <v>279</v>
+      </c>
+      <c r="E39">
+        <v>100</v>
+      </c>
+      <c r="F39">
+        <v>120</v>
+      </c>
+      <c r="G39">
+        <v>86</v>
+      </c>
+      <c r="H39">
+        <v>120</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="K39" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="L39" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="M39" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="O39" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="P39" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q39" s="18" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A40" s="20" t="s">
         <v>262</v>
       </c>
@@ -3929,11 +3988,28 @@
         <v>200</v>
       </c>
       <c r="D40" t="s">
-        <v>30</v>
-      </c>
-      <c r="I40" s="7"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+        <v>279</v>
+      </c>
+      <c r="E40">
+        <v>100</v>
+      </c>
+      <c r="F40">
+        <v>120</v>
+      </c>
+      <c r="G40">
+        <v>86</v>
+      </c>
+      <c r="H40">
+        <v>120</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="K40" s="17" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A41" s="20" t="s">
         <v>263</v>
       </c>
@@ -3943,15 +4019,35 @@
       <c r="C41" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="I41" s="7"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D41" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="E41">
+        <v>100</v>
+      </c>
+      <c r="F41">
+        <v>120</v>
+      </c>
+      <c r="G41">
+        <v>86</v>
+      </c>
+      <c r="H41">
+        <v>120</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="K41" s="17" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A42" s="20"/>
       <c r="B42" s="4"/>
       <c r="C42" s="20"/>
       <c r="I42" s="7"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="s">
         <v>128</v>
       </c>
@@ -3966,7 +4062,7 @@
       </c>
       <c r="I43" s="7"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A44" s="20" t="s">
         <v>271</v>
       </c>
@@ -3981,7 +4077,7 @@
       </c>
       <c r="I44" s="7"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A45" s="20" t="s">
         <v>272</v>
       </c>
@@ -3993,13 +4089,13 @@
       </c>
       <c r="I45" s="7"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="20"/>
       <c r="I46" s="7"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="s">
         <v>141</v>
       </c>
@@ -4014,7 +4110,7 @@
       </c>
       <c r="I47" s="7"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A48" s="20" t="s">
         <v>269</v>
       </c>
@@ -4029,7 +4125,7 @@
       </c>
       <c r="I48" s="7"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A49" s="20" t="s">
         <v>270</v>
       </c>
@@ -4041,31 +4137,31 @@
       </c>
       <c r="I49" s="7"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="20"/>
       <c r="I50" s="7"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A51" s="4"/>
       <c r="B51" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B52" s="5"/>
       <c r="I52" s="7"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B53" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B54" s="22"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="B57" s="5" t="s">
         <v>33</v>
       </c>
@@ -4078,16 +4174,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -4124,16 +4220,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4169,16 +4265,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4214,20 +4310,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView topLeftCell="A38" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.4609375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>112</v>
       </c>
@@ -4238,7 +4334,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -4252,7 +4348,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>114</v>
       </c>
@@ -4266,7 +4362,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>115</v>
       </c>
@@ -4280,7 +4376,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -4291,7 +4387,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>117</v>
       </c>
@@ -4302,7 +4398,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>118</v>
       </c>
@@ -4316,7 +4412,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>119</v>
       </c>
@@ -4330,7 +4426,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>120</v>
       </c>
@@ -4341,7 +4437,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>121</v>
       </c>
@@ -4352,7 +4448,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>122</v>
       </c>
@@ -4363,7 +4459,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>123</v>
       </c>
@@ -4374,7 +4470,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>124</v>
       </c>
@@ -4385,7 +4481,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="68" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>125</v>
       </c>
@@ -4396,7 +4492,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>126</v>
       </c>
@@ -4407,7 +4503,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>127</v>
       </c>
@@ -4418,7 +4514,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>128</v>
       </c>
@@ -4429,7 +4525,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>129</v>
       </c>
@@ -4440,7 +4536,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>130</v>
       </c>
@@ -4451,7 +4547,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>131</v>
       </c>
@@ -4462,7 +4558,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>132</v>
       </c>
@@ -4473,7 +4569,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>133</v>
       </c>
@@ -4484,7 +4580,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>134</v>
       </c>
@@ -4495,7 +4591,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>135</v>
       </c>
@@ -4506,7 +4602,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>136</v>
       </c>
@@ -4517,7 +4613,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>137</v>
       </c>
@@ -4528,7 +4624,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>138</v>
       </c>
@@ -4539,7 +4635,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>139</v>
       </c>
@@ -4550,7 +4646,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>140</v>
       </c>
@@ -4561,7 +4657,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>141</v>
       </c>
@@ -4572,7 +4668,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>142</v>
       </c>
@@ -4583,7 +4679,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>143</v>
       </c>
@@ -4594,7 +4690,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>144</v>
       </c>
@@ -4608,7 +4704,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>145</v>
       </c>
@@ -4619,7 +4715,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="51" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>146</v>
       </c>
@@ -4630,7 +4726,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>147</v>
       </c>
@@ -4641,7 +4737,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>148</v>
       </c>
@@ -4652,7 +4748,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>149</v>
       </c>
@@ -4663,7 +4759,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>150</v>
       </c>
@@ -4674,7 +4770,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>151</v>
       </c>
@@ -4685,7 +4781,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>152</v>
       </c>
@@ -4696,7 +4792,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>153</v>
       </c>
@@ -4707,7 +4803,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="34" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>154</v>
       </c>

</xml_diff>

<commit_message>
finished unit tests, updated report
</commit_message>
<xml_diff>
--- a/TeamXXReport.xlsx
+++ b/TeamXXReport.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="285">
   <si>
     <t xml:space="preserve">Initials</t>
   </si>
@@ -651,7 +651,7 @@
     <t xml:space="preserve">test_multipleBirths</t>
   </si>
   <si>
-    <t xml:space="preserve">13-21</t>
+    <t xml:space="preserve">50-59</t>
   </si>
   <si>
     <t xml:space="preserve">T32.01</t>
@@ -666,6 +666,21 @@
     <t xml:space="preserve">Compare birth dates </t>
   </si>
   <si>
+    <t xml:space="preserve">us16.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sameLastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9-51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testNames</t>
+  </si>
+  <si>
+    <t xml:space="preserve">62-71</t>
+  </si>
+  <si>
     <t xml:space="preserve">T16.01</t>
   </si>
   <si>
@@ -696,7 +711,7 @@
     <t xml:space="preserve">testDeaths</t>
   </si>
   <si>
-    <t xml:space="preserve">26-37</t>
+    <t xml:space="preserve">73-82</t>
   </si>
   <si>
     <t xml:space="preserve">T29.01</t>
@@ -708,7 +723,7 @@
     <t xml:space="preserve">T29.02</t>
   </si>
   <si>
-    <t xml:space="preserve">Store name of deceased</t>
+    <t xml:space="preserve">Store name if deceased</t>
   </si>
   <si>
     <t xml:space="preserve">Review Results</t>
@@ -1076,7 +1091,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1257,11 +1272,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="73382460"/>
-        <c:axId val="22813388"/>
+        <c:axId val="33713875"/>
+        <c:axId val="80896723"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="73382460"/>
+        <c:axId val="33713875"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1293,14 +1308,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22813388"/>
+        <c:crossAx val="80896723"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22813388"/>
+        <c:axId val="80896723"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1342,7 +1357,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73382460"/>
+        <c:crossAx val="33713875"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1474,11 +1489,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="94516346"/>
-        <c:axId val="29495774"/>
+        <c:axId val="50735632"/>
+        <c:axId val="44907627"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="94516346"/>
+        <c:axId val="50735632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1510,14 +1525,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29495774"/>
+        <c:crossAx val="44907627"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="29495774"/>
+        <c:axId val="44907627"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1559,7 +1574,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94516346"/>
+        <c:crossAx val="50735632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1597,9 +1612,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>396720</xdr:colOff>
+      <xdr:colOff>396000</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>24480</xdr:rowOff>
+      <xdr:rowOff>23760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1608,7 +1623,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="3627720"/>
-        <a:ext cx="4916160" cy="2670480"/>
+        <a:ext cx="4915440" cy="2669760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1627,9 +1642,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>947160</xdr:colOff>
+      <xdr:colOff>946440</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>159840</xdr:rowOff>
+      <xdr:rowOff>159120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1639,7 +1654,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1342080" y="1511280"/>
-          <a:ext cx="1243800" cy="629640"/>
+          <a:ext cx="1243080" cy="628920"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1726,9 +1741,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>498240</xdr:colOff>
+      <xdr:colOff>497520</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>41400</xdr:rowOff>
+      <xdr:rowOff>40680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1738,7 +1753,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5581080" y="1485720"/>
-          <a:ext cx="1272240" cy="536760"/>
+          <a:ext cx="1271520" cy="536040"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1806,9 +1821,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>63000</xdr:colOff>
+      <xdr:colOff>62280</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>134280</xdr:rowOff>
+      <xdr:rowOff>133560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1818,7 +1833,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2878200" y="1316520"/>
-          <a:ext cx="1094400" cy="798840"/>
+          <a:ext cx="1093680" cy="798120"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1886,9 +1901,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>506880</xdr:colOff>
+      <xdr:colOff>506160</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>83520</xdr:rowOff>
+      <xdr:rowOff>82800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1898,7 +1913,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4007520" y="1638000"/>
-          <a:ext cx="408960" cy="426600"/>
+          <a:ext cx="408240" cy="425880"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1985,9 +2000,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>91800</xdr:colOff>
+      <xdr:colOff>91080</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>100440</xdr:rowOff>
+      <xdr:rowOff>99720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1997,7 +2012,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4480200" y="1337400"/>
-          <a:ext cx="1079280" cy="744120"/>
+          <a:ext cx="1078560" cy="743400"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -2065,9 +2080,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>625320</xdr:colOff>
+      <xdr:colOff>624600</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>142920</xdr:rowOff>
+      <xdr:rowOff>142200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2077,7 +2092,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5733360" y="5126400"/>
-          <a:ext cx="1247040" cy="629640"/>
+          <a:ext cx="1246320" cy="628920"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -2150,9 +2165,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>396720</xdr:colOff>
+      <xdr:colOff>396000</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>24480</xdr:rowOff>
+      <xdr:rowOff>23760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2161,7 +2176,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="948240" y="1481400"/>
-        <a:ext cx="5346720" cy="2670480"/>
+        <a:ext cx="5346000" cy="2669760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3261,10 +3276,10 @@
   </sheetPr>
   <dimension ref="A1:Q58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F45" activeCellId="0" sqref="F45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="Q49" activeCellId="0" sqref="Q49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3829,7 +3844,7 @@
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>57</v>
       </c>
@@ -3876,7 +3891,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
         <v>208</v>
       </c>
@@ -3907,8 +3922,11 @@
       <c r="K40" s="13" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L40" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
         <v>210</v>
       </c>
@@ -3938,6 +3956,9 @@
       </c>
       <c r="K41" s="13" t="s">
         <v>202</v>
+      </c>
+      <c r="L41" s="18" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3945,7 +3966,7 @@
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>52</v>
       </c>
@@ -3956,7 +3977,7 @@
         <v>25</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="E43" s="0" t="n">
         <v>45</v>
@@ -3964,19 +3985,46 @@
       <c r="F43" s="0" t="n">
         <v>120</v>
       </c>
-    </row>
-    <row r="44" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G43" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="H43" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="K43" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="L43" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="M43" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="O43" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="P43" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q43" s="13" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>45</v>
@@ -3984,19 +4032,34 @@
       <c r="F44" s="0" t="n">
         <v>120</v>
       </c>
+      <c r="G44" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="H44" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="K44" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="L44" s="13" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D45" s="0" t="s">
-        <v>39</v>
+      <c r="D45" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="E45" s="0" t="n">
         <v>45</v>
@@ -4004,25 +4067,55 @@
       <c r="F45" s="0" t="n">
         <v>120</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G45" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="H45" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="K45" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="L45" s="13" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="E46" s="0" t="n">
         <v>45</v>
       </c>
       <c r="F46" s="0" t="n">
         <v>120</v>
+      </c>
+      <c r="G46" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="H46" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="K46" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="L46" s="13" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4030,7 +4123,7 @@
       <c r="B47" s="1"/>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>54</v>
       </c>
@@ -4059,30 +4152,30 @@
         <v>201</v>
       </c>
       <c r="K48" s="13" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="L48" s="13" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="M48" s="13" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="O48" s="13" t="s">
         <v>205</v>
       </c>
       <c r="P48" s="13" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="Q48" s="13" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>25</v>
@@ -4106,19 +4199,25 @@
         <v>201</v>
       </c>
       <c r="K49" s="13" t="s">
-        <v>218</v>
+        <v>223</v>
+      </c>
+      <c r="L49" s="13" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="D50" s="0" t="s">
+        <v>56</v>
+      </c>
       <c r="E50" s="0" t="n">
         <v>10</v>
       </c>
@@ -4135,7 +4234,10 @@
         <v>201</v>
       </c>
       <c r="K50" s="13" t="s">
-        <v>218</v>
+        <v>223</v>
+      </c>
+      <c r="L50" s="13" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4146,7 +4248,7 @@
     <row r="52" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1"/>
       <c r="B52" s="14" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4154,7 +4256,7 @@
     </row>
     <row r="54" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="14" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4162,7 +4264,7 @@
     </row>
     <row r="58" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="14" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -4371,7 +4473,7 @@
         <v>34</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4382,10 +4484,10 @@
         <v>38</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="30.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4396,10 +4498,10 @@
         <v>41</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="30.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4410,10 +4512,10 @@
         <v>43</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4424,7 +4526,7 @@
         <v>45</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="30.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4435,7 +4537,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="30.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4446,10 +4548,10 @@
         <v>49</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="59" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4460,10 +4562,10 @@
         <v>196</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4474,7 +4576,7 @@
         <v>60</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4485,7 +4587,7 @@
         <v>62</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4496,18 +4598,18 @@
         <v>64</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4518,7 +4620,7 @@
         <v>66</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="68" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4529,7 +4631,7 @@
         <v>68</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4540,7 +4642,7 @@
         <v>70</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="30.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4551,7 +4653,7 @@
         <v>72</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4562,7 +4664,7 @@
         <v>53</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="30.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4573,7 +4675,7 @@
         <v>74</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4584,7 +4686,7 @@
         <v>76</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4595,7 +4697,7 @@
         <v>78</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4606,7 +4708,7 @@
         <v>80</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4617,7 +4719,7 @@
         <v>82</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4628,7 +4730,7 @@
         <v>84</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4639,7 +4741,7 @@
         <v>86</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4650,7 +4752,7 @@
         <v>88</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4661,7 +4763,7 @@
         <v>90</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="136" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4672,7 +4774,7 @@
         <v>92</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4683,7 +4785,7 @@
         <v>94</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4694,7 +4796,7 @@
         <v>96</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4705,7 +4807,7 @@
         <v>55</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4716,7 +4818,7 @@
         <v>98</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="30.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4727,7 +4829,7 @@
         <v>100</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4738,10 +4840,10 @@
         <v>58</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4752,7 +4854,7 @@
         <v>102</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4763,7 +4865,7 @@
         <v>104</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4774,7 +4876,7 @@
         <v>106</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="30.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4785,7 +4887,7 @@
         <v>108</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4796,7 +4898,7 @@
         <v>110</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4807,7 +4909,7 @@
         <v>112</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4818,18 +4920,18 @@
         <v>114</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="34" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4840,7 +4942,7 @@
         <v>116</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4851,7 +4953,7 @@
         <v>118</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Sprint1 a bit
</commit_message>
<xml_diff>
--- a/TeamXXReport.xlsx
+++ b/TeamXXReport.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
-  <workbookPr date1904="1" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chloequinto/Documents/SSW_555_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StevensUser\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5695A467-99D5-A747-8B89-C5C6EED20CB6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3100" yWindow="460" windowWidth="23120" windowHeight="16840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3100" yWindow="460" windowWidth="23120" windowHeight="16840" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
     <sheet name="Sprint4" sheetId="8" r:id="rId8"/>
     <sheet name="Stories" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="298">
   <si>
     <t>Initials</t>
   </si>
@@ -924,16 +923,24 @@
   </si>
   <si>
     <t>86-91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>us03.birthBeforeDeath</t>
+  </si>
+  <si>
+    <t>us03.py</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1012,7 +1019,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1464,6 +1471,9 @@
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2551,23 +2561,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.84375" customWidth="1"/>
+    <col min="2" max="2" width="15.69140625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="4" max="5" width="20.4609375" customWidth="1"/>
     <col min="6" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2584,7 +2594,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2601,7 +2611,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2618,7 +2628,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2635,7 +2645,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -2652,7 +2662,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
@@ -2669,7 +2679,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D9" s="1" t="s">
         <v>30</v>
       </c>
@@ -2679,12 +2689,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D5" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2692,24 +2702,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="6.69140625" customWidth="1"/>
+    <col min="2" max="2" width="9.69140625" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="6.69140625" customWidth="1"/>
+    <col min="5" max="5" width="7.69140625" customWidth="1"/>
     <col min="6" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -2726,7 +2736,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2743,7 +2753,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2760,7 +2770,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2777,7 +2787,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2794,7 +2804,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2811,7 +2821,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2828,7 +2838,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2845,7 +2855,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2862,7 +2872,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2879,7 +2889,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2896,7 +2906,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2910,7 +2920,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2924,7 +2934,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2938,7 +2948,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2952,7 +2962,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2966,7 +2976,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2980,7 +2990,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2994,7 +3004,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2</v>
       </c>
@@ -3008,7 +3018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2</v>
       </c>
@@ -3022,7 +3032,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2</v>
       </c>
@@ -3036,7 +3046,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>3</v>
       </c>
@@ -3050,7 +3060,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>3</v>
       </c>
@@ -3064,7 +3074,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>3</v>
       </c>
@@ -3078,7 +3088,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>3</v>
       </c>
@@ -3092,7 +3102,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>3</v>
       </c>
@@ -3106,7 +3116,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3</v>
       </c>
@@ -3120,7 +3130,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>3</v>
       </c>
@@ -3134,7 +3144,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>3</v>
       </c>
@@ -3148,7 +3158,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>3</v>
       </c>
@@ -3162,7 +3172,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>3</v>
       </c>
@@ -3176,7 +3186,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>4</v>
       </c>
@@ -3190,7 +3200,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>4</v>
       </c>
@@ -3204,7 +3214,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>4</v>
       </c>
@@ -3218,7 +3228,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>4</v>
       </c>
@@ -3232,7 +3242,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>4</v>
       </c>
@@ -3246,7 +3256,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>4</v>
       </c>
@@ -3260,7 +3270,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>4</v>
       </c>
@@ -3274,7 +3284,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>4</v>
       </c>
@@ -3288,7 +3298,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>4</v>
       </c>
@@ -3302,7 +3312,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>4</v>
       </c>
@@ -3323,55 +3333,55 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="6" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="9.4609375" customWidth="1"/>
+    <col min="3" max="3" width="15.84375" customWidth="1"/>
+    <col min="4" max="4" width="12.3046875" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" style="6" customWidth="1"/>
     <col min="7" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
@@ -3394,7 +3404,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>130</v>
       </c>
@@ -3410,7 +3420,7 @@
       <c r="F15" s="10"/>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>131</v>
       </c>
@@ -3435,7 +3445,7 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>132</v>
       </c>
@@ -3460,7 +3470,7 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>133</v>
       </c>
@@ -3485,7 +3495,7 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>134</v>
       </c>
@@ -3518,25 +3528,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5" style="5" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="6" customWidth="1"/>
+    <col min="1" max="1" width="17.4609375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="16.69140625" customWidth="1"/>
+    <col min="3" max="3" width="12.4609375" customWidth="1"/>
+    <col min="4" max="4" width="7.15234375" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" style="6" customWidth="1"/>
     <col min="7" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>124</v>
       </c>
@@ -3556,7 +3566,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>135</v>
       </c>
@@ -3567,26 +3577,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>136</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
       </c>
       <c r="F3" s="6" t="e">
         <f>(D3-D2)/E3*60</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>139</v>
       </c>
@@ -3599,38 +3615,38 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q58"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="2" max="2" width="37.33203125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.84375" customWidth="1"/>
+    <col min="2" max="2" width="37.3046875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="7.3046875" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" customWidth="1"/>
-    <col min="7" max="7" width="8.5" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="6" max="6" width="9.15234375" customWidth="1"/>
+    <col min="7" max="7" width="8.4609375" customWidth="1"/>
+    <col min="8" max="8" width="9.3046875" customWidth="1"/>
     <col min="9" max="9" width="11" style="5" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="11.5" style="13"/>
-    <col min="12" max="12" width="19.1640625" style="13" customWidth="1"/>
+    <col min="11" max="11" width="11.4609375" style="13"/>
+    <col min="12" max="12" width="19.15234375" style="13" customWidth="1"/>
     <col min="13" max="13" width="13" style="13" customWidth="1"/>
-    <col min="14" max="14" width="1.83203125" style="13" customWidth="1"/>
+    <col min="14" max="14" width="1.84375" style="13" customWidth="1"/>
     <col min="15" max="15" width="17" style="13" customWidth="1"/>
-    <col min="16" max="16" width="21.83203125" style="13" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="13" customWidth="1"/>
+    <col min="16" max="16" width="21.84375" style="13" customWidth="1"/>
+    <col min="17" max="17" width="10.15234375" style="13" customWidth="1"/>
     <col min="18" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -3677,7 +3693,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -3694,10 +3710,10 @@
         <v>150</v>
       </c>
       <c r="F2">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="G2">
-        <v>120</v>
+        <v>190</v>
       </c>
       <c r="H2">
         <v>90</v>
@@ -3724,7 +3740,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>158</v>
       </c>
@@ -3737,8 +3753,20 @@
       <c r="D3" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+      <c r="E3">
+        <v>30</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <v>190</v>
+      </c>
+      <c r="H3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>160</v>
       </c>
@@ -3751,8 +3779,26 @@
       <c r="D4" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+      <c r="E4">
+        <v>30</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="G4">
+        <v>190</v>
+      </c>
+      <c r="H4">
+        <v>90</v>
+      </c>
+      <c r="J4">
+        <v>150</v>
+      </c>
+      <c r="L4" s="13">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>162</v>
       </c>
@@ -3765,8 +3811,26 @@
       <c r="D5" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+      <c r="E5">
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <v>190</v>
+      </c>
+      <c r="H5">
+        <v>90</v>
+      </c>
+      <c r="J5">
+        <v>150</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>164</v>
       </c>
@@ -3779,8 +3843,23 @@
       <c r="D6" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E6">
+        <v>30</v>
+      </c>
+      <c r="F6">
+        <v>20</v>
+      </c>
+      <c r="G6">
+        <v>190</v>
+      </c>
+      <c r="H6">
+        <v>90</v>
+      </c>
+      <c r="J6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>166</v>
       </c>
@@ -3793,14 +3872,26 @@
       <c r="D7" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E7">
+        <v>30</v>
+      </c>
+      <c r="F7">
+        <v>20</v>
+      </c>
+      <c r="G7">
+        <v>190</v>
+      </c>
+      <c r="H7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>168</v>
       </c>
@@ -3814,10 +3905,10 @@
         <v>55</v>
       </c>
       <c r="E9">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="F9">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="K9" s="18" t="s">
         <v>152</v>
@@ -3838,7 +3929,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>173</v>
       </c>
@@ -3851,8 +3942,14 @@
       <c r="D10" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+      <c r="E10">
+        <v>20</v>
+      </c>
+      <c r="F10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>175</v>
       </c>
@@ -3865,8 +3962,14 @@
       <c r="D11" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+      <c r="E11">
+        <v>20</v>
+      </c>
+      <c r="F11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>176</v>
       </c>
@@ -3879,12 +3982,18 @@
       <c r="D12" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="E12">
+        <v>40</v>
+      </c>
+      <c r="F12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>41</v>
       </c>
@@ -3897,11 +4006,29 @@
       <c r="D14" t="s">
         <v>55</v>
       </c>
+      <c r="E14">
+        <v>80</v>
+      </c>
+      <c r="F14">
+        <v>60</v>
+      </c>
+      <c r="G14">
+        <v>100</v>
+      </c>
+      <c r="H14">
+        <v>120</v>
+      </c>
+      <c r="I14" s="5">
+        <v>41687</v>
+      </c>
       <c r="K14" s="18" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+        <v>297</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>178</v>
       </c>
@@ -3914,9 +4041,29 @@
       <c r="D15" t="s">
         <v>55</v>
       </c>
-      <c r="K15" s="18"/>
-    </row>
-    <row r="16" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+      <c r="E15">
+        <v>20</v>
+      </c>
+      <c r="F15">
+        <v>20</v>
+      </c>
+      <c r="G15">
+        <v>40</v>
+      </c>
+      <c r="H15">
+        <v>50</v>
+      </c>
+      <c r="I15" s="5">
+        <v>41687</v>
+      </c>
+      <c r="K15" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>179</v>
       </c>
@@ -3929,9 +4076,29 @@
       <c r="D16" t="s">
         <v>55</v>
       </c>
-      <c r="K16" s="18"/>
-    </row>
-    <row r="17" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E16">
+        <v>20</v>
+      </c>
+      <c r="F16">
+        <v>20</v>
+      </c>
+      <c r="G16">
+        <v>40</v>
+      </c>
+      <c r="H16">
+        <v>50</v>
+      </c>
+      <c r="I16" s="5">
+        <v>41687</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>181</v>
       </c>
@@ -3944,14 +4111,34 @@
       <c r="D17" t="s">
         <v>55</v>
       </c>
-      <c r="K17" s="18"/>
-    </row>
-    <row r="18" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E17">
+        <v>40</v>
+      </c>
+      <c r="F17">
+        <v>20</v>
+      </c>
+      <c r="G17">
+        <v>20</v>
+      </c>
+      <c r="H17">
+        <v>20</v>
+      </c>
+      <c r="I17" s="5">
+        <v>41687</v>
+      </c>
+      <c r="K17" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="4"/>
       <c r="C18" s="3"/>
       <c r="K18" s="18"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>43</v>
       </c>
@@ -3964,11 +4151,17 @@
       <c r="D19" t="s">
         <v>55</v>
       </c>
+      <c r="E19">
+        <v>80</v>
+      </c>
+      <c r="F19">
+        <v>60</v>
+      </c>
       <c r="K19" s="18" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>183</v>
       </c>
@@ -3981,9 +4174,15 @@
       <c r="D20" t="s">
         <v>55</v>
       </c>
+      <c r="E20">
+        <v>20</v>
+      </c>
+      <c r="F20">
+        <v>20</v>
+      </c>
       <c r="K20" s="18"/>
     </row>
-    <row r="21" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>184</v>
       </c>
@@ -3996,9 +4195,15 @@
       <c r="D21" t="s">
         <v>55</v>
       </c>
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <v>20</v>
+      </c>
       <c r="K21" s="18"/>
     </row>
-    <row r="22" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>185</v>
       </c>
@@ -4011,14 +4216,20 @@
       <c r="D22" t="s">
         <v>55</v>
       </c>
+      <c r="E22">
+        <v>40</v>
+      </c>
+      <c r="F22">
+        <v>20</v>
+      </c>
       <c r="K22" s="18"/>
     </row>
-    <row r="23" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4"/>
       <c r="C23" s="3"/>
       <c r="K23" s="18"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>45</v>
       </c>
@@ -4031,11 +4242,17 @@
       <c r="D24" t="s">
         <v>55</v>
       </c>
+      <c r="E24">
+        <v>80</v>
+      </c>
+      <c r="F24">
+        <v>60</v>
+      </c>
       <c r="K24" s="18" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>186</v>
       </c>
@@ -4048,9 +4265,15 @@
       <c r="D25" t="s">
         <v>55</v>
       </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25">
+        <v>20</v>
+      </c>
       <c r="K25" s="18"/>
     </row>
-    <row r="26" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>187</v>
       </c>
@@ -4063,9 +4286,15 @@
       <c r="D26" t="s">
         <v>55</v>
       </c>
+      <c r="E26">
+        <v>20</v>
+      </c>
+      <c r="F26">
+        <v>20</v>
+      </c>
       <c r="K26" s="18"/>
     </row>
-    <row r="27" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>188</v>
       </c>
@@ -4078,14 +4307,20 @@
       <c r="D27" t="s">
         <v>55</v>
       </c>
+      <c r="E27">
+        <v>40</v>
+      </c>
+      <c r="F27">
+        <v>20</v>
+      </c>
       <c r="K27" s="18"/>
     </row>
-    <row r="28" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="4"/>
       <c r="C28" s="3"/>
       <c r="K28" s="18"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>47</v>
       </c>
@@ -4098,11 +4333,17 @@
       <c r="D29" t="s">
         <v>55</v>
       </c>
+      <c r="E29">
+        <v>80</v>
+      </c>
+      <c r="F29">
+        <v>60</v>
+      </c>
       <c r="K29" s="18" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>190</v>
       </c>
@@ -4115,9 +4356,15 @@
       <c r="D30" t="s">
         <v>55</v>
       </c>
+      <c r="E30">
+        <v>20</v>
+      </c>
+      <c r="F30">
+        <v>20</v>
+      </c>
       <c r="K30" s="18"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>191</v>
       </c>
@@ -4130,9 +4377,15 @@
       <c r="D31" s="3" t="s">
         <v>55</v>
       </c>
+      <c r="E31">
+        <v>20</v>
+      </c>
+      <c r="F31">
+        <v>20</v>
+      </c>
       <c r="K31" s="18"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>192</v>
       </c>
@@ -4145,15 +4398,21 @@
       <c r="D32" s="3" t="s">
         <v>55</v>
       </c>
+      <c r="E32">
+        <v>40</v>
+      </c>
+      <c r="F32">
+        <v>20</v>
+      </c>
       <c r="K32" s="18"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="K33" s="18"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>194</v>
       </c>
@@ -4167,7 +4426,7 @@
         <v>55</v>
       </c>
       <c r="E34">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="F34">
         <v>60</v>
@@ -4200,7 +4459,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>196</v>
       </c>
@@ -4214,10 +4473,10 @@
         <v>55</v>
       </c>
       <c r="E35">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="F35">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="G35">
         <v>25</v>
@@ -4238,7 +4497,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>197</v>
       </c>
@@ -4252,10 +4511,10 @@
         <v>55</v>
       </c>
       <c r="E36">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="F36">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="G36">
         <v>25</v>
@@ -4276,7 +4535,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>198</v>
       </c>
@@ -4290,10 +4549,10 @@
         <v>55</v>
       </c>
       <c r="E37">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="F37">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="G37">
         <v>25</v>
@@ -4314,12 +4573,12 @@
         <v>292</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>56</v>
       </c>
@@ -4336,7 +4595,7 @@
         <v>100</v>
       </c>
       <c r="F39">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="G39">
         <v>86</v>
@@ -4366,7 +4625,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>207</v>
       </c>
@@ -4380,10 +4639,10 @@
         <v>55</v>
       </c>
       <c r="E40">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="F40">
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="G40">
         <v>86</v>
@@ -4401,7 +4660,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>209</v>
       </c>
@@ -4415,10 +4674,10 @@
         <v>55</v>
       </c>
       <c r="E41">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="F41">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="G41">
         <v>86</v>
@@ -4436,12 +4695,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="1"/>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>51</v>
       </c>
@@ -4455,7 +4714,7 @@
         <v>55</v>
       </c>
       <c r="E43">
-        <v>45</v>
+        <v>120</v>
       </c>
       <c r="F43">
         <v>120</v>
@@ -4488,7 +4747,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>216</v>
       </c>
@@ -4502,10 +4761,10 @@
         <v>55</v>
       </c>
       <c r="E44">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F44">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="G44">
         <v>42</v>
@@ -4523,7 +4782,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>218</v>
       </c>
@@ -4537,10 +4796,10 @@
         <v>55</v>
       </c>
       <c r="E45">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F45">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="G45">
         <v>42</v>
@@ -4558,7 +4817,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>220</v>
       </c>
@@ -4572,10 +4831,10 @@
         <v>55</v>
       </c>
       <c r="E46">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F46">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="G46">
         <v>42</v>
@@ -4593,12 +4852,12 @@
         <v>212</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>53</v>
       </c>
@@ -4612,10 +4871,10 @@
         <v>55</v>
       </c>
       <c r="E48">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="F48">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G48">
         <v>6</v>
@@ -4645,7 +4904,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>227</v>
       </c>
@@ -4659,10 +4918,10 @@
         <v>55</v>
       </c>
       <c r="E49">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F49">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G49">
         <v>6</v>
@@ -4680,7 +4939,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>229</v>
       </c>
@@ -4694,10 +4953,10 @@
         <v>55</v>
       </c>
       <c r="E50">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F50">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G50">
         <v>6</v>
@@ -4715,29 +4974,29 @@
         <v>223</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="3"/>
     </row>
-    <row r="52" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="14" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B53" s="14"/>
     </row>
-    <row r="54" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B54" s="14" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B55" s="4"/>
     </row>
-    <row r="58" spans="1:12" ht="14" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B58" s="14" t="s">
         <v>233</v>
       </c>
@@ -4749,19 +5008,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -4797,19 +5056,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -4845,19 +5104,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -4893,22 +5152,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="28.1640625" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="12" customWidth="1"/>
+    <col min="2" max="2" width="28.15234375" customWidth="1"/>
+    <col min="3" max="3" width="49.4609375" style="12" customWidth="1"/>
     <col min="4" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -4919,7 +5178,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="85" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -4933,7 +5192,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -4947,7 +5206,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -4961,7 +5220,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="85" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -4972,7 +5231,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -4983,7 +5242,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -4997,7 +5256,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="136" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -5011,7 +5270,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="85" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -5022,7 +5281,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="85" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -5033,7 +5292,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="102" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -5044,7 +5303,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="68" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>248</v>
       </c>
@@ -5055,7 +5314,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="119" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="75" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -5066,7 +5325,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="170" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="105" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>66</v>
       </c>
@@ -5077,7 +5336,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="68" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -5088,7 +5347,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -5099,7 +5358,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -5110,7 +5369,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -5121,7 +5380,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -5132,7 +5391,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -5143,7 +5402,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="68" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -5154,7 +5413,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="68" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>80</v>
       </c>
@@ -5165,7 +5424,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="68" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>82</v>
       </c>
@@ -5176,7 +5435,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="102" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="60" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -5187,7 +5446,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="119" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="75" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>86</v>
       </c>
@@ -5198,7 +5457,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="85" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -5209,7 +5468,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="356" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="195" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>90</v>
       </c>
@@ -5220,7 +5479,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>92</v>
       </c>
@@ -5231,7 +5490,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="68" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>94</v>
       </c>
@@ -5242,7 +5501,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -5253,7 +5512,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>96</v>
       </c>
@@ -5264,7 +5523,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="68" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>98</v>
       </c>
@@ -5275,7 +5534,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="51" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>56</v>
       </c>
@@ -5289,7 +5548,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="85" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>100</v>
       </c>
@@ -5300,7 +5559,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="102" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4" ht="60" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>102</v>
       </c>
@@ -5311,7 +5570,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="68" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>104</v>
       </c>
@@ -5322,7 +5581,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="68" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:4" ht="45" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>106</v>
       </c>
@@ -5333,7 +5592,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="85" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="60" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>108</v>
       </c>
@@ -5344,7 +5603,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="85" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>110</v>
       </c>
@@ -5355,7 +5614,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="85" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" ht="60" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>112</v>
       </c>
@@ -5366,7 +5625,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="68" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>279</v>
       </c>
@@ -5377,7 +5636,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="68" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>114</v>
       </c>
@@ -5388,7 +5647,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="85" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:4" ht="60" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>116</v>
       </c>

</xml_diff>

<commit_message>
Updated Sprint 2 Page
</commit_message>
<xml_diff>
--- a/TeamXXReport.xlsx
+++ b/TeamXXReport.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11109"/>
-  <workbookPr date1904="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr date1904="1" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/SSW_555_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StevensUser\Desktop\SSW_555_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB97594-ADC3-8A44-A8DF-B0935DBC127E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
     <sheet name="Sprint4" sheetId="8" r:id="rId8"/>
     <sheet name="Stories" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="391">
   <si>
     <t>Initials</t>
   </si>
@@ -1124,15 +1123,102 @@
   </si>
   <si>
     <t>Store date</t>
+  </si>
+  <si>
+    <t>us10.py</t>
+  </si>
+  <si>
+    <t>us10.checkIndividuals</t>
+  </si>
+  <si>
+    <t>44-56</t>
+  </si>
+  <si>
+    <t>157-163</t>
+  </si>
+  <si>
+    <t>us15.py</t>
+  </si>
+  <si>
+    <t>us15.checkFewerThan15</t>
+  </si>
+  <si>
+    <t>lines 4-15</t>
+  </si>
+  <si>
+    <t>us21.py</t>
+  </si>
+  <si>
+    <t>us21.checkGenderForRole</t>
+  </si>
+  <si>
+    <t>98-106</t>
+  </si>
+  <si>
+    <t>testGenderForRole</t>
+  </si>
+  <si>
+    <t>testUS10</t>
+  </si>
+  <si>
+    <t>141-146</t>
+  </si>
+  <si>
+    <t>us22.py</t>
+  </si>
+  <si>
+    <t>us22.uniqueIDs</t>
+  </si>
+  <si>
+    <t>Lines 6-39</t>
+  </si>
+  <si>
+    <t>us26.py</t>
+  </si>
+  <si>
+    <t>us26.corrEntries</t>
+  </si>
+  <si>
+    <t>Lines 9-50</t>
+  </si>
+  <si>
+    <t>us31.py</t>
+  </si>
+  <si>
+    <t>us31.checkForLivingSingle</t>
+  </si>
+  <si>
+    <t>Lines 6-14</t>
+  </si>
+  <si>
+    <t>testUS31</t>
+  </si>
+  <si>
+    <t>147-155</t>
+  </si>
+  <si>
+    <t>us35.py</t>
+  </si>
+  <si>
+    <t>us35.RecentBirths</t>
+  </si>
+  <si>
+    <t>134-147</t>
+  </si>
+  <si>
+    <t>testRecentBirths</t>
+  </si>
+  <si>
+    <t>136-139</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="m/d"/>
-    <numFmt numFmtId="177" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="m/d"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -1216,7 +1302,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1224,13 +1310,13 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1243,7 +1329,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1255,16 +1341,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1350,7 +1438,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -1406,7 +1494,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1484,7 +1572,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1508,7 +1596,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="69682197"/>
@@ -1558,7 +1646,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="70594587"/>
@@ -1597,7 +1685,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -1745,7 +1833,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="68853745"/>
@@ -1796,7 +1884,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="63599449"/>
@@ -2736,19 +2824,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E12" activeCellId="1" sqref="I50 E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.84375" customWidth="1"/>
+    <col min="2" max="2" width="15.69140625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="4" max="5" width="20.4609375" customWidth="1"/>
     <col min="6" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2865,12 +2953,12 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D5" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2878,20 +2966,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A14" sqref="A14:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="6.69140625" customWidth="1"/>
+    <col min="2" max="2" width="9.69140625" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="6.69140625" customWidth="1"/>
+    <col min="5" max="5" width="7.69140625" customWidth="1"/>
     <col min="6" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2912,7 +3000,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2929,7 +3017,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3510,21 +3598,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E7" activeCellId="1" sqref="I50 E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="6" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="9.4609375" customWidth="1"/>
+    <col min="3" max="3" width="15.84375" customWidth="1"/>
+    <col min="4" max="4" width="12.3046875" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" style="6" customWidth="1"/>
     <col min="7" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3706,21 +3794,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="F3" activeCellId="1" sqref="I50 F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="17.5" style="5" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="6" customWidth="1"/>
+    <col min="1" max="1" width="17.4609375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="16.69140625" customWidth="1"/>
+    <col min="3" max="3" width="12.4609375" customWidth="1"/>
+    <col min="4" max="4" width="7.15234375" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" style="6" customWidth="1"/>
     <col min="7" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3800,38 +3888,38 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="L1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="I50" sqref="I50"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1:Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="2" max="2" width="37.33203125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.84375" customWidth="1"/>
+    <col min="2" max="2" width="37.3046875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="7.3046875" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" customWidth="1"/>
-    <col min="7" max="7" width="8.5" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="6" max="6" width="9.15234375" customWidth="1"/>
+    <col min="7" max="7" width="8.4609375" customWidth="1"/>
+    <col min="8" max="8" width="9.3046875" customWidth="1"/>
     <col min="9" max="9" width="11" style="5" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="11.5" style="13"/>
+    <col min="11" max="11" width="11.4609375" style="13"/>
     <col min="12" max="12" width="24" style="13" customWidth="1"/>
     <col min="13" max="13" width="13" style="13" customWidth="1"/>
-    <col min="14" max="14" width="1.83203125" style="13" customWidth="1"/>
+    <col min="14" max="14" width="1.84375" style="13" customWidth="1"/>
     <col min="15" max="15" width="17" style="13" customWidth="1"/>
-    <col min="16" max="16" width="21.83203125" style="13" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="13" customWidth="1"/>
+    <col min="16" max="16" width="21.84375" style="13" customWidth="1"/>
+    <col min="17" max="17" width="10.15234375" style="13" customWidth="1"/>
     <col min="18" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -3878,7 +3966,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="14">
+    <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -3925,7 +4013,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="14">
+    <row r="3" spans="1:17">
       <c r="A3" s="3" t="s">
         <v>158</v>
       </c>
@@ -3964,7 +4052,7 @@
       <c r="P3" s="18"/>
       <c r="Q3" s="18"/>
     </row>
-    <row r="4" spans="1:17" ht="14">
+    <row r="4" spans="1:17">
       <c r="A4" s="3" t="s">
         <v>160</v>
       </c>
@@ -4003,7 +4091,7 @@
       <c r="P4" s="18"/>
       <c r="Q4" s="18"/>
     </row>
-    <row r="5" spans="1:17" ht="14">
+    <row r="5" spans="1:17">
       <c r="A5" s="3" t="s">
         <v>162</v>
       </c>
@@ -4042,7 +4130,7 @@
       <c r="P5" s="18"/>
       <c r="Q5" s="18"/>
     </row>
-    <row r="6" spans="1:17" ht="14">
+    <row r="6" spans="1:17">
       <c r="A6" s="3" t="s">
         <v>164</v>
       </c>
@@ -4126,7 +4214,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:17" ht="14">
+    <row r="9" spans="1:17">
       <c r="A9" s="1" t="s">
         <v>168</v>
       </c>
@@ -4173,7 +4261,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="14">
+    <row r="10" spans="1:17">
       <c r="A10" s="3" t="s">
         <v>174</v>
       </c>
@@ -4212,7 +4300,7 @@
       <c r="P10" s="18"/>
       <c r="Q10" s="18"/>
     </row>
-    <row r="11" spans="1:17" ht="14">
+    <row r="11" spans="1:17">
       <c r="A11" s="3" t="s">
         <v>176</v>
       </c>
@@ -4251,7 +4339,7 @@
       <c r="P11" s="18"/>
       <c r="Q11" s="18"/>
     </row>
-    <row r="12" spans="1:17" ht="14">
+    <row r="12" spans="1:17">
       <c r="A12" s="3" t="s">
         <v>177</v>
       </c>
@@ -4341,7 +4429,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="14">
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>184</v>
       </c>
@@ -4377,7 +4465,7 @@
       </c>
       <c r="O15" s="18"/>
     </row>
-    <row r="16" spans="1:17" ht="14">
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
         <v>185</v>
       </c>
@@ -4501,7 +4589,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="14">
+    <row r="20" spans="1:17">
       <c r="A20" s="3" t="s">
         <v>194</v>
       </c>
@@ -4536,7 +4624,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="14">
+    <row r="21" spans="1:17">
       <c r="A21" s="3" t="s">
         <v>195</v>
       </c>
@@ -4658,7 +4746,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="14">
+    <row r="25" spans="1:17">
       <c r="A25" s="3" t="s">
         <v>202</v>
       </c>
@@ -4693,7 +4781,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="14">
+    <row r="26" spans="1:17">
       <c r="A26" s="3" t="s">
         <v>203</v>
       </c>
@@ -5484,7 +5572,7 @@
       <c r="B51" s="1"/>
       <c r="C51" s="3"/>
     </row>
-    <row r="52" spans="1:12" ht="14">
+    <row r="52" spans="1:12">
       <c r="A52" s="1"/>
       <c r="B52" s="14" t="s">
         <v>261</v>
@@ -5493,7 +5581,7 @@
     <row r="53" spans="1:12">
       <c r="B53" s="14"/>
     </row>
-    <row r="54" spans="1:12" ht="14">
+    <row r="54" spans="1:12">
       <c r="B54" s="14" t="s">
         <v>262</v>
       </c>
@@ -5512,7 +5600,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="14">
+    <row r="58" spans="1:12">
       <c r="B58" s="14" t="s">
         <v>266</v>
       </c>
@@ -5543,21 +5631,27 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="K31" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="Q38" sqref="Q38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="1025" width="11" customWidth="1"/>
+    <col min="3" max="11" width="11" customWidth="1"/>
+    <col min="12" max="12" width="21.07421875" customWidth="1"/>
+    <col min="13" max="13" width="13.07421875" customWidth="1"/>
+    <col min="14" max="14" width="2.765625" customWidth="1"/>
+    <col min="15" max="15" width="11" customWidth="1"/>
+    <col min="16" max="16" width="15.69140625" customWidth="1"/>
+    <col min="17" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -5585,8 +5679,27 @@
       <c r="I1" s="15" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="K1" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" s="22" t="s">
         <v>58</v>
       </c>
@@ -5597,7 +5710,7 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>321</v>
+        <v>39</v>
       </c>
       <c r="E2">
         <v>120</v>
@@ -5605,8 +5718,35 @@
       <c r="F2">
         <v>75</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="G2">
+        <v>63</v>
+      </c>
+      <c r="H2">
+        <v>60</v>
+      </c>
+      <c r="I2" s="9">
+        <v>42063</v>
+      </c>
+      <c r="K2" t="s">
+        <v>362</v>
+      </c>
+      <c r="L2" t="s">
+        <v>363</v>
+      </c>
+      <c r="M2" t="s">
+        <v>364</v>
+      </c>
+      <c r="O2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P2" t="s">
+        <v>373</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>322</v>
       </c>
@@ -5614,7 +5754,7 @@
         <v>324</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>321</v>
+        <v>39</v>
       </c>
       <c r="E3">
         <v>60</v>
@@ -5622,8 +5762,20 @@
       <c r="F3">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="G3">
+        <v>33</v>
+      </c>
+      <c r="H3">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s">
+        <v>362</v>
+      </c>
+      <c r="L3" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="23" t="s">
         <v>323</v>
       </c>
@@ -5631,7 +5783,7 @@
         <v>325</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>321</v>
+        <v>39</v>
       </c>
       <c r="E4">
         <v>60</v>
@@ -5639,8 +5791,20 @@
       <c r="F4">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="G4">
+        <v>30</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
+      </c>
+      <c r="K4" t="s">
+        <v>362</v>
+      </c>
+      <c r="L4" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" s="22" t="s">
         <v>60</v>
       </c>
@@ -5660,7 +5824,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:17">
       <c r="A7" s="23" t="s">
         <v>326</v>
       </c>
@@ -5674,7 +5838,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:17">
       <c r="A8" s="23" t="s">
         <v>327</v>
       </c>
@@ -5688,7 +5852,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:17">
       <c r="A10" s="22" t="s">
         <v>62</v>
       </c>
@@ -5699,7 +5863,7 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>321</v>
+        <v>39</v>
       </c>
       <c r="E10">
         <v>110</v>
@@ -5707,39 +5871,90 @@
       <c r="F10">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="G10">
+        <v>18</v>
+      </c>
+      <c r="H10">
+        <v>15</v>
+      </c>
+      <c r="I10" s="9">
+        <v>42063</v>
+      </c>
+      <c r="K10" t="s">
+        <v>366</v>
+      </c>
+      <c r="L10" t="s">
+        <v>367</v>
+      </c>
+      <c r="M10" s="24" t="s">
+        <v>368</v>
+      </c>
+      <c r="O10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" s="23" t="s">
         <v>330</v>
       </c>
       <c r="B11" s="23" t="s">
         <v>332</v>
       </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
       <c r="E11">
         <v>60</v>
       </c>
       <c r="F11">
         <v>60</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="G11">
+        <v>14</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="K11" t="s">
+        <v>366</v>
+      </c>
+      <c r="L11" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" s="23" t="s">
         <v>331</v>
       </c>
       <c r="B12" s="23" t="s">
         <v>333</v>
       </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
       <c r="E12">
         <v>50</v>
       </c>
       <c r="F12">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>5</v>
+      </c>
+      <c r="K12" t="s">
+        <v>366</v>
+      </c>
+      <c r="L12" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" s="22"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:17">
       <c r="A14" s="22" t="s">
         <v>64</v>
       </c>
@@ -5759,7 +5974,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:17">
       <c r="A15" s="23" t="s">
         <v>334</v>
       </c>
@@ -5773,7 +5988,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:17">
       <c r="A17" s="22" t="s">
         <v>66</v>
       </c>
@@ -5793,7 +6008,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:17">
       <c r="A18" s="23" t="s">
         <v>336</v>
       </c>
@@ -5807,7 +6022,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:17">
       <c r="A19" s="23" t="s">
         <v>339</v>
       </c>
@@ -5821,7 +6036,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:17">
       <c r="A20" s="23" t="s">
         <v>340</v>
       </c>
@@ -5835,7 +6050,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:17">
       <c r="A22" s="22" t="s">
         <v>68</v>
       </c>
@@ -5846,7 +6061,7 @@
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>321</v>
+        <v>39</v>
       </c>
       <c r="E22">
         <v>130</v>
@@ -5854,36 +6069,93 @@
       <c r="F22">
         <v>120</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22">
+        <v>114</v>
+      </c>
+      <c r="H22">
+        <v>100</v>
+      </c>
+      <c r="I22" s="9">
+        <v>42063</v>
+      </c>
+      <c r="K22" t="s">
+        <v>369</v>
+      </c>
+      <c r="L22" t="s">
+        <v>370</v>
+      </c>
+      <c r="M22" t="s">
+        <v>371</v>
+      </c>
+      <c r="O22" t="s">
+        <v>155</v>
+      </c>
+      <c r="P22" t="s">
+        <v>372</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23" s="23" t="s">
         <v>342</v>
       </c>
       <c r="B23" s="23" t="s">
         <v>343</v>
       </c>
+      <c r="D23" t="s">
+        <v>39</v>
+      </c>
       <c r="E23">
         <v>65</v>
       </c>
       <c r="F23">
         <v>70</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23">
+        <v>57</v>
+      </c>
+      <c r="H23">
+        <v>50</v>
+      </c>
+      <c r="K23" t="s">
+        <v>369</v>
+      </c>
+      <c r="L23" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
       <c r="A24" s="23" t="s">
         <v>344</v>
       </c>
       <c r="B24" s="23" t="s">
         <v>345</v>
       </c>
+      <c r="D24" t="s">
+        <v>39</v>
+      </c>
       <c r="E24">
         <v>65</v>
       </c>
       <c r="F24">
         <v>50</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G24">
+        <v>57</v>
+      </c>
+      <c r="H24">
+        <v>50</v>
+      </c>
+      <c r="K24" t="s">
+        <v>369</v>
+      </c>
+      <c r="L24" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
       <c r="A26" s="22" t="s">
         <v>70</v>
       </c>
@@ -5894,7 +6166,7 @@
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>321</v>
+        <v>39</v>
       </c>
       <c r="E26">
         <v>100</v>
@@ -5902,36 +6174,87 @@
       <c r="F26">
         <v>110</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26">
+        <v>39</v>
+      </c>
+      <c r="H26">
+        <v>70</v>
+      </c>
+      <c r="I26" s="9">
+        <v>42063</v>
+      </c>
+      <c r="K26" t="s">
+        <v>375</v>
+      </c>
+      <c r="L26" t="s">
+        <v>376</v>
+      </c>
+      <c r="M26" s="25" t="s">
+        <v>377</v>
+      </c>
+      <c r="O26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
       <c r="A27" s="23" t="s">
         <v>346</v>
       </c>
       <c r="B27" s="23" t="s">
         <v>347</v>
       </c>
+      <c r="D27" t="s">
+        <v>39</v>
+      </c>
       <c r="E27">
         <v>60</v>
       </c>
       <c r="F27">
         <v>60</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27">
+        <v>14</v>
+      </c>
+      <c r="H27">
+        <v>35</v>
+      </c>
+      <c r="K27" t="s">
+        <v>375</v>
+      </c>
+      <c r="L27" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
       <c r="A28" s="23" t="s">
         <v>348</v>
       </c>
       <c r="B28" s="23" t="s">
         <v>349</v>
       </c>
+      <c r="D28" t="s">
+        <v>39</v>
+      </c>
       <c r="E28">
         <v>40</v>
       </c>
       <c r="F28">
         <v>50</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G28">
+        <v>15</v>
+      </c>
+      <c r="H28">
+        <v>35</v>
+      </c>
+      <c r="K28" t="s">
+        <v>375</v>
+      </c>
+      <c r="L28" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
       <c r="A30" s="22" t="s">
         <v>72</v>
       </c>
@@ -5942,7 +6265,7 @@
         <v>25</v>
       </c>
       <c r="D30" t="s">
-        <v>321</v>
+        <v>39</v>
       </c>
       <c r="E30">
         <v>100</v>
@@ -5950,22 +6273,58 @@
       <c r="F30">
         <v>100</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" s="23" customFormat="1">
+      <c r="G30">
+        <v>50</v>
+      </c>
+      <c r="H30">
+        <v>70</v>
+      </c>
+      <c r="I30" s="9">
+        <v>42063</v>
+      </c>
+      <c r="K30" t="s">
+        <v>378</v>
+      </c>
+      <c r="L30" t="s">
+        <v>379</v>
+      </c>
+      <c r="M30" t="s">
+        <v>380</v>
+      </c>
+      <c r="O30" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" s="23" customFormat="1">
       <c r="A31" s="23" t="s">
         <v>350</v>
       </c>
       <c r="B31" s="23" t="s">
         <v>351</v>
       </c>
+      <c r="D31" s="23" t="s">
+        <v>39</v>
+      </c>
       <c r="E31" s="23">
         <v>100</v>
       </c>
       <c r="F31" s="23">
         <v>100</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G31" s="23">
+        <v>50</v>
+      </c>
+      <c r="H31" s="23">
+        <v>70</v>
+      </c>
+      <c r="K31" s="23" t="s">
+        <v>378</v>
+      </c>
+      <c r="L31" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
       <c r="A33" s="22" t="s">
         <v>74</v>
       </c>
@@ -5976,7 +6335,7 @@
         <v>15</v>
       </c>
       <c r="D33" t="s">
-        <v>321</v>
+        <v>39</v>
       </c>
       <c r="E33">
         <v>80</v>
@@ -5984,50 +6343,122 @@
       <c r="F33">
         <v>75</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33">
+        <v>22</v>
+      </c>
+      <c r="H33">
+        <v>15</v>
+      </c>
+      <c r="I33" s="9">
+        <v>42063</v>
+      </c>
+      <c r="K33" t="s">
+        <v>381</v>
+      </c>
+      <c r="L33" t="s">
+        <v>382</v>
+      </c>
+      <c r="M33" t="s">
+        <v>383</v>
+      </c>
+      <c r="O33" t="s">
+        <v>155</v>
+      </c>
+      <c r="P33" t="s">
+        <v>384</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
       <c r="A34" s="23" t="s">
         <v>352</v>
       </c>
       <c r="B34" s="23" t="s">
         <v>353</v>
       </c>
+      <c r="D34" t="s">
+        <v>39</v>
+      </c>
       <c r="E34">
         <v>30</v>
       </c>
       <c r="F34">
         <v>30</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34">
+        <v>7</v>
+      </c>
+      <c r="H34">
+        <v>5</v>
+      </c>
+      <c r="K34" t="s">
+        <v>381</v>
+      </c>
+      <c r="L34" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
       <c r="A35" s="23" t="s">
         <v>354</v>
       </c>
       <c r="B35" s="23" t="s">
         <v>355</v>
       </c>
+      <c r="D35" t="s">
+        <v>39</v>
+      </c>
       <c r="E35">
         <v>30</v>
       </c>
       <c r="F35">
         <v>30</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35">
+        <v>7</v>
+      </c>
+      <c r="H35">
+        <v>5</v>
+      </c>
+      <c r="K35" t="s">
+        <v>381</v>
+      </c>
+      <c r="L35" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
       <c r="A36" s="23" t="s">
         <v>356</v>
       </c>
       <c r="B36" s="23" t="s">
         <v>357</v>
       </c>
+      <c r="D36" t="s">
+        <v>39</v>
+      </c>
       <c r="E36" s="23">
         <v>20</v>
       </c>
       <c r="F36">
         <v>15</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G36">
+        <v>8</v>
+      </c>
+      <c r="H36">
+        <v>5</v>
+      </c>
+      <c r="K36" t="s">
+        <v>381</v>
+      </c>
+      <c r="L36" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
       <c r="A38" s="22" t="s">
         <v>76</v>
       </c>
@@ -6038,7 +6469,7 @@
         <v>10</v>
       </c>
       <c r="D38" t="s">
-        <v>321</v>
+        <v>39</v>
       </c>
       <c r="E38">
         <v>80</v>
@@ -6046,33 +6477,90 @@
       <c r="F38">
         <v>75</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38">
+        <v>155</v>
+      </c>
+      <c r="H38">
+        <v>60</v>
+      </c>
+      <c r="I38" s="9">
+        <v>42063</v>
+      </c>
+      <c r="K38" t="s">
+        <v>386</v>
+      </c>
+      <c r="L38" t="s">
+        <v>387</v>
+      </c>
+      <c r="M38" t="s">
+        <v>388</v>
+      </c>
+      <c r="O38" t="s">
+        <v>155</v>
+      </c>
+      <c r="P38" t="s">
+        <v>389</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
       <c r="A39" s="23" t="s">
         <v>358</v>
       </c>
       <c r="B39" s="23" t="s">
         <v>359</v>
       </c>
+      <c r="D39" t="s">
+        <v>39</v>
+      </c>
       <c r="E39">
         <v>40</v>
       </c>
       <c r="F39">
         <v>50</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="G39">
+        <v>100</v>
+      </c>
+      <c r="H39">
+        <v>30</v>
+      </c>
+      <c r="K39" t="s">
+        <v>386</v>
+      </c>
+      <c r="L39" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17">
       <c r="A40" s="23" t="s">
         <v>360</v>
       </c>
       <c r="B40" s="23" t="s">
         <v>361</v>
       </c>
+      <c r="D40" t="s">
+        <v>39</v>
+      </c>
       <c r="E40">
         <v>40</v>
       </c>
       <c r="F40">
         <v>25</v>
+      </c>
+      <c r="G40">
+        <v>55</v>
+      </c>
+      <c r="H40">
+        <v>30</v>
+      </c>
+      <c r="K40" t="s">
+        <v>386</v>
+      </c>
+      <c r="L40" t="s">
+        <v>387</v>
       </c>
     </row>
   </sheetData>
@@ -6083,19 +6571,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C1" activeCellId="1" sqref="I50 C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -6132,19 +6620,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C1" activeCellId="1" sqref="I50 C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -6181,22 +6669,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C18" activeCellId="1" sqref="I50 C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="28.1640625" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="12" customWidth="1"/>
+    <col min="2" max="2" width="28.15234375" customWidth="1"/>
+    <col min="3" max="3" width="49.4609375" style="12" customWidth="1"/>
     <col min="4" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="14">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -6207,7 +6695,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="85">
+    <row r="2" spans="1:4" ht="45">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -6221,7 +6709,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="51">
+    <row r="3" spans="1:4" ht="30">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -6235,7 +6723,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="51">
+    <row r="4" spans="1:4" ht="30">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -6249,7 +6737,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="85">
+    <row r="5" spans="1:4" ht="60">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -6260,7 +6748,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="51">
+    <row r="6" spans="1:4" ht="30">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -6271,7 +6759,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="51">
+    <row r="7" spans="1:4" ht="30">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -6285,7 +6773,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="136">
+    <row r="8" spans="1:4" ht="75">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -6299,7 +6787,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="85">
+    <row r="9" spans="1:4" ht="60">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -6310,7 +6798,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="85">
+    <row r="10" spans="1:4" ht="45">
       <c r="A10" t="s">
         <v>104</v>
       </c>
@@ -6321,7 +6809,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="102">
+    <row r="11" spans="1:4" ht="60">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -6332,7 +6820,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="68">
+    <row r="12" spans="1:4" ht="45">
       <c r="A12" t="s">
         <v>285</v>
       </c>
@@ -6343,7 +6831,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="119">
+    <row r="13" spans="1:4" ht="75">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -6354,7 +6842,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="170">
+    <row r="14" spans="1:4" ht="105">
       <c r="A14" t="s">
         <v>82</v>
       </c>
@@ -6365,7 +6853,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="68">
+    <row r="15" spans="1:4" ht="45">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -6376,7 +6864,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="51">
+    <row r="16" spans="1:4" ht="30">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -6387,7 +6875,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="51">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -6398,7 +6886,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="51">
+    <row r="18" spans="1:3" ht="30">
       <c r="A18" t="s">
         <v>90</v>
       </c>
@@ -6409,7 +6897,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="34">
+    <row r="19" spans="1:3" ht="30">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -6420,7 +6908,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="51">
+    <row r="20" spans="1:3" ht="30">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -6431,7 +6919,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="68">
+    <row r="21" spans="1:3" ht="30">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -6442,7 +6930,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="68">
+    <row r="22" spans="1:3" ht="45">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -6453,7 +6941,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="68">
+    <row r="23" spans="1:3" ht="45">
       <c r="A23" t="s">
         <v>70</v>
       </c>
@@ -6464,7 +6952,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="85">
+    <row r="24" spans="1:3" ht="60">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -6475,7 +6963,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="102">
+    <row r="25" spans="1:3" ht="75">
       <c r="A25" t="s">
         <v>86</v>
       </c>
@@ -6486,7 +6974,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="85">
+    <row r="26" spans="1:3" ht="45">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -6497,7 +6985,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="356">
+    <row r="27" spans="1:3" ht="195">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -6508,7 +6996,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="51">
+    <row r="28" spans="1:3" ht="30">
       <c r="A28" t="s">
         <v>92</v>
       </c>
@@ -6519,7 +7007,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="68">
+    <row r="29" spans="1:3" ht="45">
       <c r="A29" t="s">
         <v>94</v>
       </c>
@@ -6530,7 +7018,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="51">
+    <row r="30" spans="1:3" ht="30">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -6541,7 +7029,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="51">
+    <row r="31" spans="1:3" ht="30">
       <c r="A31" t="s">
         <v>96</v>
       </c>
@@ -6552,7 +7040,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="68">
+    <row r="32" spans="1:3" ht="45">
       <c r="A32" t="s">
         <v>74</v>
       </c>
@@ -6563,7 +7051,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="51">
+    <row r="33" spans="1:4" ht="30">
       <c r="A33" t="s">
         <v>56</v>
       </c>
@@ -6577,7 +7065,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="85">
+    <row r="34" spans="1:4" ht="45">
       <c r="A34" t="s">
         <v>100</v>
       </c>
@@ -6588,7 +7076,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="102">
+    <row r="35" spans="1:4" ht="60">
       <c r="A35" t="s">
         <v>102</v>
       </c>
@@ -6599,7 +7087,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="68">
+    <row r="36" spans="1:4" ht="45">
       <c r="A36" t="s">
         <v>76</v>
       </c>
@@ -6610,7 +7098,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="68">
+    <row r="37" spans="1:4" ht="45">
       <c r="A37" t="s">
         <v>106</v>
       </c>
@@ -6621,7 +7109,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="85">
+    <row r="38" spans="1:4" ht="60">
       <c r="A38" t="s">
         <v>108</v>
       </c>
@@ -6632,7 +7120,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="85">
+    <row r="39" spans="1:4" ht="45">
       <c r="A39" t="s">
         <v>110</v>
       </c>
@@ -6643,7 +7131,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="85">
+    <row r="40" spans="1:4" ht="60">
       <c r="A40" t="s">
         <v>112</v>
       </c>
@@ -6654,7 +7142,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="68">
+    <row r="41" spans="1:4" ht="45">
       <c r="A41" t="s">
         <v>316</v>
       </c>
@@ -6665,7 +7153,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="68">
+    <row r="42" spans="1:4" ht="45">
       <c r="A42" t="s">
         <v>114</v>
       </c>
@@ -6676,7 +7164,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="85">
+    <row r="43" spans="1:4" ht="60">
       <c r="A43" t="s">
         <v>116</v>
       </c>

</xml_diff>

<commit_message>
Finished Excel for Sprint 3
</commit_message>
<xml_diff>
--- a/TeamXXReport.xlsx
+++ b/TeamXXReport.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11109"/>
-  <workbookPr date1904="1" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr date1904="1" autoCompressPictures="0" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/SSW_555_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StevensUser\Desktop\SSW_555_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4119AD1F-7C38-D847-9292-6FAAF211A1FC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="460" windowWidth="27980" windowHeight="16000" tabRatio="500" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="460" windowWidth="27980" windowHeight="16000" tabRatio="500" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
     <sheet name="Sprint4" sheetId="8" r:id="rId8"/>
     <sheet name="Stories" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="546">
   <si>
     <t>T21.01</t>
   </si>
@@ -1594,15 +1593,162 @@
   <si>
     <t>185-191</t>
     <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>us12.py</t>
+  </si>
+  <si>
+    <t>us12.checkForOldParents</t>
+  </si>
+  <si>
+    <t>18-64</t>
+  </si>
+  <si>
+    <t>testUS12</t>
+  </si>
+  <si>
+    <t>331-335</t>
+  </si>
+  <si>
+    <t>us28.py</t>
+  </si>
+  <si>
+    <t>us28.orderSiblings</t>
+  </si>
+  <si>
+    <t>Lines 7-36</t>
+  </si>
+  <si>
+    <t>testUS28</t>
+  </si>
+  <si>
+    <t>311-315</t>
+  </si>
+  <si>
+    <t>us33.py</t>
+  </si>
+  <si>
+    <t>us33.checkForOrphans</t>
+  </si>
+  <si>
+    <t>Lines 6-33</t>
+  </si>
+  <si>
+    <t>testUS33</t>
+  </si>
+  <si>
+    <t>276-280</t>
+  </si>
+  <si>
+    <t>us36.py</t>
+  </si>
+  <si>
+    <t>us36.recentDeaths</t>
+  </si>
+  <si>
+    <t>Lines 11-26</t>
+  </si>
+  <si>
+    <t>testUS36</t>
+  </si>
+  <si>
+    <t>317-322</t>
+  </si>
+  <si>
+    <t>us38.py</t>
+  </si>
+  <si>
+    <t>us38.upcomingBirthdays</t>
+  </si>
+  <si>
+    <t>testUS38</t>
+  </si>
+  <si>
+    <t>324-329</t>
+  </si>
+  <si>
+    <t>us42.py</t>
+  </si>
+  <si>
+    <t>us42.rejectBadDates</t>
+  </si>
+  <si>
+    <t>47-81</t>
+  </si>
+  <si>
+    <t>test42</t>
+  </si>
+  <si>
+    <t>271-274</t>
+  </si>
+  <si>
+    <t>T13.01</t>
+  </si>
+  <si>
+    <t>T13.02</t>
+  </si>
+  <si>
+    <t>Compare Birthdates</t>
+  </si>
+  <si>
+    <t>T17.01</t>
+  </si>
+  <si>
+    <t>T17.02</t>
+  </si>
+  <si>
+    <t>Get spouses</t>
+  </si>
+  <si>
+    <t>Check if related</t>
+  </si>
+  <si>
+    <t>T20.01</t>
+  </si>
+  <si>
+    <t>T20.02</t>
+  </si>
+  <si>
+    <t>Check if related (aunts and uncles)</t>
+  </si>
+  <si>
+    <t>T24.01</t>
+  </si>
+  <si>
+    <t>T24.02</t>
+  </si>
+  <si>
+    <t>Get each family</t>
+  </si>
+  <si>
+    <t>Check for same marriage date and spouse names</t>
+  </si>
+  <si>
+    <t>T34.01</t>
+  </si>
+  <si>
+    <t>T34.02</t>
+  </si>
+  <si>
+    <t>Get spouse ages at marriage</t>
+  </si>
+  <si>
+    <t>Check if one spouse twice as old</t>
+  </si>
+  <si>
+    <t>Pair Programming</t>
+  </si>
+  <si>
+    <t>Not sufficiently planning for user stories that interact with others</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="m/d"/>
-    <numFmt numFmtId="177" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="m/d"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -1709,13 +1855,13 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1728,7 +1874,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1740,7 +1886,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
     </xf>
@@ -1751,15 +1897,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="58" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
@@ -1845,7 +1991,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1908,7 +2054,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41065</c:v>
@@ -1986,7 +2132,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2010,7 +2156,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="344433960"/>
@@ -2060,7 +2206,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="344345464"/>
@@ -2099,7 +2245,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
-  <c:lang val="zh-CN"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2196,6 +2342,9 @@
                 <c:pt idx="2">
                   <c:v>20</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2257,7 +2406,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="344410552"/>
@@ -2308,7 +2457,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="344411272"/>
@@ -3248,19 +3397,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="E12" activeCellId="1" sqref="I50 E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.84375" customWidth="1"/>
+    <col min="2" max="2" width="15.69140625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="5" width="20.33203125" customWidth="1"/>
+    <col min="4" max="5" width="20.3046875" customWidth="1"/>
     <col min="6" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3377,12 +3526,12 @@
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D5" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <extLst>
@@ -3394,20 +3543,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView topLeftCell="A34" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="B38" sqref="B38:D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="6.69140625" customWidth="1"/>
+    <col min="2" max="2" width="9.69140625" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="6.69140625" customWidth="1"/>
+    <col min="5" max="5" width="7.69140625" customWidth="1"/>
     <col min="6" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3428,7 +3577,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3445,7 +3594,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3781,6 +3930,9 @@
       <c r="D26" t="s">
         <v>291</v>
       </c>
+      <c r="E26" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27">
@@ -3795,6 +3947,9 @@
       <c r="D27" t="s">
         <v>291</v>
       </c>
+      <c r="E27" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28">
@@ -3809,6 +3964,9 @@
       <c r="D28" t="s">
         <v>296</v>
       </c>
+      <c r="E28" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29">
@@ -3823,6 +3981,9 @@
       <c r="D29" t="s">
         <v>306</v>
       </c>
+      <c r="E29" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30">
@@ -3837,6 +3998,9 @@
       <c r="D30" t="s">
         <v>296</v>
       </c>
+      <c r="E30" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31">
@@ -3851,6 +4015,9 @@
       <c r="D31" t="s">
         <v>301</v>
       </c>
+      <c r="E31" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32">
@@ -3865,8 +4032,11 @@
       <c r="D32" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>3</v>
       </c>
@@ -3879,8 +4049,11 @@
       <c r="D33" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>3</v>
       </c>
@@ -3893,8 +4066,11 @@
       <c r="D34" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>3</v>
       </c>
@@ -3907,8 +4083,11 @@
       <c r="D35" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E35" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>4</v>
       </c>
@@ -3922,35 +4101,35 @@
         <v>291</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>359</v>
+        <v>371</v>
       </c>
       <c r="C39" t="s">
-        <v>360</v>
+        <v>372</v>
       </c>
       <c r="D39" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>383</v>
+        <v>359</v>
       </c>
       <c r="C40" t="s">
-        <v>384</v>
+        <v>360</v>
       </c>
       <c r="D40" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>4</v>
       </c>
@@ -3961,88 +4140,88 @@
         <v>366</v>
       </c>
       <c r="D41" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>4</v>
       </c>
       <c r="B42" t="s">
-        <v>347</v>
+        <v>367</v>
       </c>
       <c r="C42" t="s">
-        <v>348</v>
+        <v>368</v>
       </c>
       <c r="D42" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>4</v>
       </c>
       <c r="B43" t="s">
-        <v>389</v>
+        <v>369</v>
       </c>
       <c r="C43" t="s">
-        <v>390</v>
+        <v>370</v>
       </c>
       <c r="D43" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:5">
       <c r="A44">
         <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="C44" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="D44" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45">
         <v>4</v>
       </c>
       <c r="B45" t="s">
-        <v>210</v>
+        <v>383</v>
       </c>
       <c r="C45" t="s">
-        <v>211</v>
+        <v>384</v>
       </c>
       <c r="D45" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46">
         <v>4</v>
       </c>
       <c r="B46" t="s">
-        <v>371</v>
+        <v>389</v>
       </c>
       <c r="C46" t="s">
-        <v>372</v>
+        <v>390</v>
       </c>
       <c r="D46" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47">
         <v>4</v>
       </c>
       <c r="B47" t="s">
-        <v>369</v>
+        <v>210</v>
       </c>
       <c r="C47" t="s">
-        <v>370</v>
+        <v>211</v>
       </c>
       <c r="D47" t="s">
         <v>301</v>
@@ -4061,21 +4240,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="E7" activeCellId="1" sqref="I50 E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="9.3046875" customWidth="1"/>
+    <col min="3" max="3" width="15.84375" customWidth="1"/>
+    <col min="4" max="4" width="12.3046875" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.3046875" style="6" customWidth="1"/>
     <col min="7" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4261,21 +4440,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.5" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="20.84375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="16.69140625" customWidth="1"/>
+    <col min="3" max="3" width="20.4609375" customWidth="1"/>
+    <col min="4" max="4" width="7.15234375" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.3046875" style="6" customWidth="1"/>
     <col min="7" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4355,6 +4534,22 @@
     <row r="5" spans="1:6">
       <c r="A5" s="5" t="s">
         <v>236</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>632</v>
+      </c>
+      <c r="E5">
+        <v>615</v>
+      </c>
+      <c r="F5" s="6">
+        <f>(D3+D4+D5-D2)/(E3+E4+E5)*60</f>
+        <v>57.769911504424776</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -4375,38 +4570,38 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="L1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="2" max="2" width="37.33203125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.84375" customWidth="1"/>
+    <col min="2" max="2" width="37.3046875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="7.3046875" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="6" max="6" width="9.15234375" customWidth="1"/>
+    <col min="7" max="7" width="8.3046875" customWidth="1"/>
+    <col min="8" max="8" width="9.3046875" customWidth="1"/>
     <col min="9" max="9" width="11" style="5" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" style="13"/>
+    <col min="11" max="11" width="8.84375" style="13"/>
     <col min="12" max="12" width="24" style="13" customWidth="1"/>
     <col min="13" max="13" width="13" style="13" customWidth="1"/>
-    <col min="14" max="14" width="1.83203125" style="13" customWidth="1"/>
+    <col min="14" max="14" width="1.84375" style="13" customWidth="1"/>
     <col min="15" max="15" width="17" style="13" customWidth="1"/>
-    <col min="16" max="16" width="21.83203125" style="13" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="13" customWidth="1"/>
+    <col min="16" max="16" width="21.84375" style="13" customWidth="1"/>
+    <col min="17" max="17" width="10.15234375" style="13" customWidth="1"/>
     <col min="18" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>314</v>
       </c>
@@ -4453,7 +4648,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="14">
+    <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
         <v>318</v>
       </c>
@@ -4500,7 +4695,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="14">
+    <row r="3" spans="1:17">
       <c r="A3" s="3" t="s">
         <v>253</v>
       </c>
@@ -4539,7 +4734,7 @@
       <c r="P3" s="18"/>
       <c r="Q3" s="18"/>
     </row>
-    <row r="4" spans="1:17" ht="14">
+    <row r="4" spans="1:17">
       <c r="A4" s="3" t="s">
         <v>255</v>
       </c>
@@ -4578,7 +4773,7 @@
       <c r="P4" s="18"/>
       <c r="Q4" s="18"/>
     </row>
-    <row r="5" spans="1:17" ht="14">
+    <row r="5" spans="1:17">
       <c r="A5" s="3" t="s">
         <v>257</v>
       </c>
@@ -4617,7 +4812,7 @@
       <c r="P5" s="18"/>
       <c r="Q5" s="18"/>
     </row>
-    <row r="6" spans="1:17" ht="14">
+    <row r="6" spans="1:17">
       <c r="A6" s="3" t="s">
         <v>259</v>
       </c>
@@ -4701,7 +4896,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:17" ht="14">
+    <row r="9" spans="1:17">
       <c r="A9" s="1" t="s">
         <v>263</v>
       </c>
@@ -4748,7 +4943,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="14">
+    <row r="10" spans="1:17">
       <c r="A10" s="3" t="s">
         <v>266</v>
       </c>
@@ -4787,7 +4982,7 @@
       <c r="P10" s="18"/>
       <c r="Q10" s="18"/>
     </row>
-    <row r="11" spans="1:17" ht="14">
+    <row r="11" spans="1:17">
       <c r="A11" s="3" t="s">
         <v>268</v>
       </c>
@@ -4826,7 +5021,7 @@
       <c r="P11" s="18"/>
       <c r="Q11" s="18"/>
     </row>
-    <row r="12" spans="1:17" ht="14">
+    <row r="12" spans="1:17">
       <c r="A12" s="3" t="s">
         <v>269</v>
       </c>
@@ -4916,7 +5111,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="14">
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>276</v>
       </c>
@@ -4952,7 +5147,7 @@
       </c>
       <c r="O15" s="18"/>
     </row>
-    <row r="16" spans="1:17" ht="14">
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
         <v>277</v>
       </c>
@@ -5076,7 +5271,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="14">
+    <row r="20" spans="1:17">
       <c r="A20" s="3" t="s">
         <v>124</v>
       </c>
@@ -5111,7 +5306,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="14">
+    <row r="21" spans="1:17">
       <c r="A21" s="3" t="s">
         <v>125</v>
       </c>
@@ -5233,7 +5428,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="14">
+    <row r="25" spans="1:17">
       <c r="A25" s="3" t="s">
         <v>132</v>
       </c>
@@ -5268,7 +5463,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="14">
+    <row r="26" spans="1:17">
       <c r="A26" s="3" t="s">
         <v>133</v>
       </c>
@@ -6059,7 +6254,7 @@
       <c r="B51" s="1"/>
       <c r="C51" s="3"/>
     </row>
-    <row r="52" spans="1:12" ht="14">
+    <row r="52" spans="1:12">
       <c r="A52" s="1"/>
       <c r="B52" s="14" t="s">
         <v>191</v>
@@ -6068,7 +6263,7 @@
     <row r="53" spans="1:12">
       <c r="B53" s="14"/>
     </row>
-    <row r="54" spans="1:12" ht="14">
+    <row r="54" spans="1:12">
       <c r="B54" s="14" t="s">
         <v>192</v>
       </c>
@@ -6087,7 +6282,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="14">
+    <row r="58" spans="1:12">
       <c r="B58" s="14" t="s">
         <v>196</v>
       </c>
@@ -6122,27 +6317,27 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="P37" sqref="P37"/>
+    <sheetView topLeftCell="A39" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="24.5" customWidth="1"/>
-    <col min="13" max="13" width="13.1640625" customWidth="1"/>
-    <col min="14" max="14" width="2.6640625" customWidth="1"/>
+    <col min="12" max="12" width="24.4609375" customWidth="1"/>
+    <col min="13" max="13" width="13.15234375" customWidth="1"/>
+    <col min="14" max="14" width="2.69140625" customWidth="1"/>
     <col min="15" max="15" width="11" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" customWidth="1"/>
+    <col min="16" max="16" width="15.69140625" customWidth="1"/>
     <col min="17" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>314</v>
       </c>
@@ -7243,7 +7438,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="14">
+    <row r="42" spans="1:17">
       <c r="B42" s="14" t="s">
         <v>191</v>
       </c>
@@ -7251,7 +7446,7 @@
     <row r="43" spans="1:17">
       <c r="B43" s="14"/>
     </row>
-    <row r="44" spans="1:17" ht="14">
+    <row r="44" spans="1:17">
       <c r="B44" s="14" t="s">
         <v>192</v>
       </c>
@@ -7286,7 +7481,7 @@
     <row r="49" spans="2:3">
       <c r="B49" s="12"/>
     </row>
-    <row r="50" spans="2:3" ht="14">
+    <row r="50" spans="2:3">
       <c r="B50" s="14" t="s">
         <v>196</v>
       </c>
@@ -7319,27 +7514,27 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:Q42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="37.5" customWidth="1"/>
+    <col min="2" max="2" width="37.4609375" customWidth="1"/>
     <col min="3" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="17.5" customWidth="1"/>
-    <col min="13" max="13" width="18.1640625" customWidth="1"/>
+    <col min="12" max="12" width="28.23046875" customWidth="1"/>
+    <col min="13" max="13" width="18.15234375" customWidth="1"/>
     <col min="14" max="15" width="11" customWidth="1"/>
-    <col min="16" max="16" width="18.83203125" customWidth="1"/>
+    <col min="16" max="16" width="18.84375" customWidth="1"/>
     <col min="17" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="14">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>314</v>
       </c>
@@ -7397,8 +7592,8 @@
       <c r="C2" s="28" t="s">
         <v>291</v>
       </c>
-      <c r="D2" s="28" t="s">
-        <v>80</v>
+      <c r="D2" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E2">
         <v>45</v>
@@ -7442,8 +7637,8 @@
         <v>402</v>
       </c>
       <c r="C3" s="28"/>
-      <c r="D3" s="28" t="s">
-        <v>80</v>
+      <c r="D3" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E3">
         <v>10</v>
@@ -7475,8 +7670,8 @@
         <v>404</v>
       </c>
       <c r="C4" s="28"/>
-      <c r="D4" s="28" t="s">
-        <v>80</v>
+      <c r="D4" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E4">
         <v>30</v>
@@ -7508,8 +7703,8 @@
         <v>406</v>
       </c>
       <c r="C5" s="28"/>
-      <c r="D5" s="28" t="s">
-        <v>80</v>
+      <c r="D5" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E5">
         <v>5</v>
@@ -7543,8 +7738,8 @@
       <c r="C7" s="28" t="s">
         <v>291</v>
       </c>
-      <c r="D7" s="28" t="s">
-        <v>80</v>
+      <c r="D7" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E7">
         <v>25</v>
@@ -7588,8 +7783,8 @@
         <v>410</v>
       </c>
       <c r="C8" s="28"/>
-      <c r="D8" s="28" t="s">
-        <v>80</v>
+      <c r="D8" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E8">
         <v>10</v>
@@ -7621,8 +7816,8 @@
         <v>411</v>
       </c>
       <c r="C9" s="28"/>
-      <c r="D9" s="28" t="s">
-        <v>80</v>
+      <c r="D9" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -7654,8 +7849,8 @@
         <v>412</v>
       </c>
       <c r="C10" s="28"/>
-      <c r="D10" s="28" t="s">
-        <v>80</v>
+      <c r="D10" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E10">
         <v>5</v>
@@ -7689,14 +7884,41 @@
       <c r="C12" s="28" t="s">
         <v>296</v>
       </c>
-      <c r="D12" s="28" t="s">
-        <v>80</v>
+      <c r="D12" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E12">
         <v>30</v>
       </c>
       <c r="F12">
         <v>45</v>
+      </c>
+      <c r="G12">
+        <v>70</v>
+      </c>
+      <c r="H12">
+        <v>45</v>
+      </c>
+      <c r="I12" s="9">
+        <v>42098</v>
+      </c>
+      <c r="K12" t="s">
+        <v>497</v>
+      </c>
+      <c r="L12" t="s">
+        <v>498</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="O12" t="s">
+        <v>252</v>
+      </c>
+      <c r="P12" t="s">
+        <v>500</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="13" spans="1:17" s="28" customFormat="1">
@@ -7706,14 +7928,29 @@
       <c r="B13" s="28" t="s">
         <v>410</v>
       </c>
-      <c r="D13" s="28" t="s">
-        <v>80</v>
+      <c r="D13" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E13" s="28">
         <v>10</v>
       </c>
       <c r="F13" s="28">
         <v>10</v>
+      </c>
+      <c r="G13" s="28">
+        <v>35</v>
+      </c>
+      <c r="H13" s="3">
+        <v>30</v>
+      </c>
+      <c r="K13" t="s">
+        <v>497</v>
+      </c>
+      <c r="L13" t="s">
+        <v>498</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="14" spans="1:17" s="28" customFormat="1">
@@ -7723,14 +7960,29 @@
       <c r="B14" s="28" t="s">
         <v>415</v>
       </c>
-      <c r="D14" s="28" t="s">
-        <v>80</v>
+      <c r="D14" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E14" s="28">
         <v>20</v>
       </c>
       <c r="F14" s="28">
         <v>35</v>
+      </c>
+      <c r="G14" s="3">
+        <v>35</v>
+      </c>
+      <c r="H14" s="3">
+        <v>15</v>
+      </c>
+      <c r="K14" t="s">
+        <v>497</v>
+      </c>
+      <c r="L14" t="s">
+        <v>498</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -7743,14 +7995,41 @@
       <c r="C16" s="28" t="s">
         <v>306</v>
       </c>
-      <c r="D16" s="28" t="s">
-        <v>80</v>
+      <c r="D16" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E16">
         <v>30</v>
       </c>
       <c r="F16">
         <v>40</v>
+      </c>
+      <c r="G16">
+        <v>36</v>
+      </c>
+      <c r="H16">
+        <v>35</v>
+      </c>
+      <c r="I16" s="9">
+        <v>42094</v>
+      </c>
+      <c r="K16" t="s">
+        <v>502</v>
+      </c>
+      <c r="L16" t="s">
+        <v>503</v>
+      </c>
+      <c r="M16" s="25" t="s">
+        <v>504</v>
+      </c>
+      <c r="O16" t="s">
+        <v>252</v>
+      </c>
+      <c r="P16" t="s">
+        <v>505</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="17" spans="1:17" s="28" customFormat="1">
@@ -7760,14 +8039,29 @@
       <c r="B17" s="28" t="s">
         <v>417</v>
       </c>
-      <c r="D17" s="28" t="s">
-        <v>80</v>
+      <c r="D17" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E17" s="28">
         <v>5</v>
       </c>
       <c r="F17" s="28">
         <v>5</v>
+      </c>
+      <c r="G17" s="28">
+        <v>18</v>
+      </c>
+      <c r="H17" s="3">
+        <v>17</v>
+      </c>
+      <c r="K17" t="s">
+        <v>502</v>
+      </c>
+      <c r="L17" t="s">
+        <v>503</v>
+      </c>
+      <c r="M17" s="25" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="18" spans="1:17" s="28" customFormat="1">
@@ -7777,14 +8071,29 @@
       <c r="B18" s="28" t="s">
         <v>419</v>
       </c>
-      <c r="D18" s="28" t="s">
-        <v>80</v>
+      <c r="D18" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E18" s="28">
         <v>25</v>
       </c>
       <c r="F18" s="28">
         <v>35</v>
+      </c>
+      <c r="G18" s="3">
+        <v>18</v>
+      </c>
+      <c r="H18" s="3">
+        <v>18</v>
+      </c>
+      <c r="K18" t="s">
+        <v>502</v>
+      </c>
+      <c r="L18" t="s">
+        <v>503</v>
+      </c>
+      <c r="M18" s="25" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -7797,14 +8106,41 @@
       <c r="C20" s="28" t="s">
         <v>296</v>
       </c>
-      <c r="D20" s="28" t="s">
-        <v>80</v>
+      <c r="D20" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E20">
         <v>25</v>
       </c>
       <c r="F20">
         <v>30</v>
+      </c>
+      <c r="G20">
+        <v>36</v>
+      </c>
+      <c r="H20">
+        <v>30</v>
+      </c>
+      <c r="I20" s="9">
+        <v>42092</v>
+      </c>
+      <c r="K20" t="s">
+        <v>507</v>
+      </c>
+      <c r="L20" t="s">
+        <v>508</v>
+      </c>
+      <c r="M20" s="25" t="s">
+        <v>509</v>
+      </c>
+      <c r="O20" t="s">
+        <v>252</v>
+      </c>
+      <c r="P20" t="s">
+        <v>510</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -7815,14 +8151,29 @@
         <v>421</v>
       </c>
       <c r="C21" s="28"/>
-      <c r="D21" s="28" t="s">
-        <v>80</v>
+      <c r="D21" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E21">
         <v>20</v>
       </c>
       <c r="F21">
         <v>20</v>
+      </c>
+      <c r="G21">
+        <v>25</v>
+      </c>
+      <c r="H21">
+        <v>20</v>
+      </c>
+      <c r="K21" t="s">
+        <v>507</v>
+      </c>
+      <c r="L21" t="s">
+        <v>508</v>
+      </c>
+      <c r="M21" s="25" t="s">
+        <v>509</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -7833,14 +8184,29 @@
         <v>423</v>
       </c>
       <c r="C22" s="28"/>
-      <c r="D22" s="28" t="s">
-        <v>80</v>
+      <c r="D22" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E22">
         <v>5</v>
       </c>
       <c r="F22">
         <v>10</v>
+      </c>
+      <c r="G22">
+        <v>11</v>
+      </c>
+      <c r="H22">
+        <v>10</v>
+      </c>
+      <c r="K22" t="s">
+        <v>507</v>
+      </c>
+      <c r="L22" t="s">
+        <v>508</v>
+      </c>
+      <c r="M22" s="25" t="s">
+        <v>509</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -7853,14 +8219,41 @@
       <c r="C24" s="28" t="s">
         <v>301</v>
       </c>
-      <c r="D24" s="28" t="s">
-        <v>80</v>
+      <c r="D24" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E24">
         <v>25</v>
       </c>
       <c r="F24">
         <v>30</v>
+      </c>
+      <c r="G24">
+        <v>31</v>
+      </c>
+      <c r="H24">
+        <v>30</v>
+      </c>
+      <c r="I24" s="9">
+        <v>42093</v>
+      </c>
+      <c r="K24" t="s">
+        <v>512</v>
+      </c>
+      <c r="L24" t="s">
+        <v>513</v>
+      </c>
+      <c r="M24" s="24" t="s">
+        <v>514</v>
+      </c>
+      <c r="O24" t="s">
+        <v>252</v>
+      </c>
+      <c r="P24" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -7871,14 +8264,32 @@
         <v>426</v>
       </c>
       <c r="C25" s="28"/>
-      <c r="D25" s="28" t="s">
-        <v>80</v>
+      <c r="D25" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E25">
         <v>5</v>
       </c>
       <c r="F25">
         <v>10</v>
+      </c>
+      <c r="G25">
+        <v>15</v>
+      </c>
+      <c r="H25">
+        <v>15</v>
+      </c>
+      <c r="K25" t="s">
+        <v>512</v>
+      </c>
+      <c r="L25" t="s">
+        <v>513</v>
+      </c>
+      <c r="M25" s="24" t="s">
+        <v>514</v>
+      </c>
+      <c r="O25" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -7889,14 +8300,32 @@
         <v>427</v>
       </c>
       <c r="C26" s="28"/>
-      <c r="D26" s="28" t="s">
-        <v>80</v>
+      <c r="D26" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E26">
         <v>20</v>
       </c>
       <c r="F26">
         <v>20</v>
+      </c>
+      <c r="G26">
+        <v>16</v>
+      </c>
+      <c r="H26">
+        <v>15</v>
+      </c>
+      <c r="K26" t="s">
+        <v>512</v>
+      </c>
+      <c r="L26" t="s">
+        <v>513</v>
+      </c>
+      <c r="M26" s="24" t="s">
+        <v>514</v>
+      </c>
+      <c r="O26" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -7909,14 +8338,41 @@
       <c r="C28" s="28" t="s">
         <v>301</v>
       </c>
-      <c r="D28" s="28" t="s">
-        <v>80</v>
+      <c r="D28" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E28">
         <v>30</v>
       </c>
       <c r="F28">
         <v>40</v>
+      </c>
+      <c r="G28">
+        <v>31</v>
+      </c>
+      <c r="H28">
+        <v>45</v>
+      </c>
+      <c r="I28" s="9">
+        <v>42100</v>
+      </c>
+      <c r="K28" t="s">
+        <v>517</v>
+      </c>
+      <c r="L28" t="s">
+        <v>518</v>
+      </c>
+      <c r="M28" s="24" t="s">
+        <v>514</v>
+      </c>
+      <c r="O28" t="s">
+        <v>252</v>
+      </c>
+      <c r="P28" t="s">
+        <v>519</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="29" spans="1:17" s="28" customFormat="1">
@@ -7926,14 +8382,32 @@
       <c r="B29" s="28" t="s">
         <v>430</v>
       </c>
-      <c r="D29" s="28" t="s">
-        <v>80</v>
+      <c r="D29" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E29" s="28">
         <v>5</v>
       </c>
       <c r="F29" s="28">
         <v>10</v>
+      </c>
+      <c r="G29" s="28">
+        <v>16</v>
+      </c>
+      <c r="H29" s="3">
+        <v>23</v>
+      </c>
+      <c r="K29" t="s">
+        <v>517</v>
+      </c>
+      <c r="L29" t="s">
+        <v>518</v>
+      </c>
+      <c r="M29" s="24" t="s">
+        <v>514</v>
+      </c>
+      <c r="O29" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="30" spans="1:17" s="28" customFormat="1">
@@ -7943,14 +8417,32 @@
       <c r="B30" s="28" t="s">
         <v>431</v>
       </c>
-      <c r="D30" s="28" t="s">
-        <v>80</v>
+      <c r="D30" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E30" s="28">
         <v>25</v>
       </c>
       <c r="F30" s="28">
         <v>30</v>
+      </c>
+      <c r="G30" s="3">
+        <v>15</v>
+      </c>
+      <c r="H30" s="3">
+        <v>22</v>
+      </c>
+      <c r="K30" t="s">
+        <v>517</v>
+      </c>
+      <c r="L30" t="s">
+        <v>518</v>
+      </c>
+      <c r="M30" s="24" t="s">
+        <v>514</v>
+      </c>
+      <c r="O30" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -7963,8 +8455,8 @@
       <c r="C32" s="28" t="s">
         <v>286</v>
       </c>
-      <c r="D32" s="28" t="s">
-        <v>80</v>
+      <c r="D32" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E32">
         <v>60</v>
@@ -8007,8 +8499,8 @@
       <c r="B33" s="28" t="s">
         <v>435</v>
       </c>
-      <c r="D33" s="28" t="s">
-        <v>80</v>
+      <c r="D33" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E33" s="28">
         <v>10</v>
@@ -8051,8 +8543,8 @@
       <c r="B34" s="28" t="s">
         <v>434</v>
       </c>
-      <c r="D34" s="28" t="s">
-        <v>80</v>
+      <c r="D34" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E34" s="28">
         <v>20</v>
@@ -8098,8 +8590,8 @@
       <c r="C36" s="28" t="s">
         <v>286</v>
       </c>
-      <c r="D36" s="28" t="s">
-        <v>80</v>
+      <c r="D36" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E36">
         <v>60</v>
@@ -8143,8 +8635,8 @@
         <v>438</v>
       </c>
       <c r="C37" s="28"/>
-      <c r="D37" s="28" t="s">
-        <v>80</v>
+      <c r="D37" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E37">
         <v>30</v>
@@ -8188,8 +8680,8 @@
         <v>439</v>
       </c>
       <c r="C38" s="28"/>
-      <c r="D38" s="28" t="s">
-        <v>80</v>
+      <c r="D38" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E38">
         <v>30</v>
@@ -8235,14 +8727,41 @@
       <c r="C40" s="28" t="s">
         <v>306</v>
       </c>
-      <c r="D40" s="28" t="s">
-        <v>80</v>
+      <c r="D40" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E40">
         <v>30</v>
       </c>
       <c r="F40">
         <v>35</v>
+      </c>
+      <c r="G40">
+        <v>81</v>
+      </c>
+      <c r="H40">
+        <v>50</v>
+      </c>
+      <c r="I40" s="9">
+        <v>42094</v>
+      </c>
+      <c r="K40" t="s">
+        <v>521</v>
+      </c>
+      <c r="L40" t="s">
+        <v>522</v>
+      </c>
+      <c r="M40" t="s">
+        <v>523</v>
+      </c>
+      <c r="O40" t="s">
+        <v>252</v>
+      </c>
+      <c r="P40" t="s">
+        <v>524</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="41" spans="1:17">
@@ -8252,14 +8771,29 @@
       <c r="B41" s="28" t="s">
         <v>441</v>
       </c>
-      <c r="D41" s="28" t="s">
-        <v>80</v>
+      <c r="D41" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E41">
         <v>25</v>
       </c>
       <c r="F41">
         <v>30</v>
+      </c>
+      <c r="G41">
+        <v>40</v>
+      </c>
+      <c r="H41">
+        <v>25</v>
+      </c>
+      <c r="L41" t="s">
+        <v>522</v>
+      </c>
+      <c r="M41" t="s">
+        <v>523</v>
+      </c>
+      <c r="O41" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="42" spans="1:17">
@@ -8269,8 +8803,8 @@
       <c r="B42" s="28" t="s">
         <v>423</v>
       </c>
-      <c r="D42" s="28" t="s">
-        <v>80</v>
+      <c r="D42" s="3" t="s">
+        <v>320</v>
       </c>
       <c r="E42">
         <v>5</v>
@@ -8278,6 +8812,82 @@
       <c r="F42">
         <v>5</v>
       </c>
+      <c r="G42">
+        <v>41</v>
+      </c>
+      <c r="H42">
+        <v>25</v>
+      </c>
+      <c r="L42" t="s">
+        <v>522</v>
+      </c>
+      <c r="M42" t="s">
+        <v>523</v>
+      </c>
+      <c r="O42" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17">
+      <c r="B44" s="14" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17">
+      <c r="B45" s="14"/>
+    </row>
+    <row r="46" spans="1:17">
+      <c r="B46" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C46" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17">
+      <c r="B47" s="4"/>
+      <c r="C47" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17">
+      <c r="B48" s="12"/>
+      <c r="C48" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="B49" s="12"/>
+      <c r="C49" s="28" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3">
+      <c r="B50" s="12"/>
+      <c r="C50" s="28" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3">
+      <c r="B51" s="12"/>
+      <c r="C51" s="3" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3">
+      <c r="B52" s="12"/>
+    </row>
+    <row r="53" spans="2:3">
+      <c r="B53" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3">
+      <c r="B54" s="12"/>
+      <c r="C54" s="28"/>
     </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
@@ -8292,20 +8902,26 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C1" activeCellId="1" sqref="I50 C1"/>
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1025" width="11" customWidth="1"/>
+    <col min="1" max="1" width="11" style="26" customWidth="1"/>
+    <col min="2" max="2" width="41.23046875" customWidth="1"/>
+    <col min="3" max="11" width="11" customWidth="1"/>
+    <col min="12" max="12" width="21.61328125" customWidth="1"/>
+    <col min="13" max="15" width="11" customWidth="1"/>
+    <col min="16" max="16" width="18.61328125" customWidth="1"/>
+    <col min="17" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:17">
+      <c r="A1" s="26" t="s">
         <v>314</v>
       </c>
       <c r="B1" s="14" t="s">
@@ -8331,11 +8947,401 @@
       </c>
       <c r="I1" s="15" t="s">
         <v>242</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="B2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2">
+        <v>35</v>
+      </c>
+      <c r="F2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="26" t="s">
+        <v>371</v>
+      </c>
+      <c r="B6" t="s">
+        <v>372</v>
+      </c>
+      <c r="C6" t="s">
+        <v>286</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6">
+        <v>50</v>
+      </c>
+      <c r="F6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8">
+        <v>35</v>
+      </c>
+      <c r="F8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="26" t="s">
+        <v>359</v>
+      </c>
+      <c r="B10" t="s">
+        <v>360</v>
+      </c>
+      <c r="C10" t="s">
+        <v>291</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10">
+        <v>60</v>
+      </c>
+      <c r="F10">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11">
+        <v>15</v>
+      </c>
+      <c r="F11">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12">
+        <v>45</v>
+      </c>
+      <c r="F12">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="26" t="s">
+        <v>365</v>
+      </c>
+      <c r="B14" t="s">
+        <v>366</v>
+      </c>
+      <c r="C14" t="s">
+        <v>296</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14">
+        <v>30</v>
+      </c>
+      <c r="F14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="26" t="s">
+        <v>367</v>
+      </c>
+      <c r="B16" t="s">
+        <v>368</v>
+      </c>
+      <c r="C16" t="s">
+        <v>286</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16">
+        <v>50</v>
+      </c>
+      <c r="F16">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17">
+        <v>20</v>
+      </c>
+      <c r="F17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18">
+        <v>30</v>
+      </c>
+      <c r="F18">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="26" t="s">
+        <v>369</v>
+      </c>
+      <c r="B20" t="s">
+        <v>370</v>
+      </c>
+      <c r="C20" t="s">
+        <v>306</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20">
+        <v>30</v>
+      </c>
+      <c r="F20">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="26" t="s">
+        <v>373</v>
+      </c>
+      <c r="B22" t="s">
+        <v>374</v>
+      </c>
+      <c r="C22" t="s">
+        <v>306</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22">
+        <v>10</v>
+      </c>
+      <c r="F22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="26" t="s">
+        <v>383</v>
+      </c>
+      <c r="B24" t="s">
+        <v>384</v>
+      </c>
+      <c r="C24" t="s">
+        <v>296</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24">
+        <v>40</v>
+      </c>
+      <c r="F24">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26">
+        <v>20</v>
+      </c>
+      <c r="F26">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="26" t="s">
+        <v>389</v>
+      </c>
+      <c r="B28" t="s">
+        <v>390</v>
+      </c>
+      <c r="C28" t="s">
+        <v>301</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E28">
+        <v>30</v>
+      </c>
+      <c r="F28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="B30" t="s">
+        <v>211</v>
+      </c>
+      <c r="C30" t="s">
+        <v>301</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30">
+        <v>30</v>
+      </c>
+      <c r="F30">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -8345,22 +9351,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView topLeftCell="A24" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="28.1640625" customWidth="1"/>
-    <col min="3" max="3" width="49.33203125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="28.15234375" customWidth="1"/>
+    <col min="3" max="3" width="49.3046875" style="12" customWidth="1"/>
     <col min="4" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="14">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>314</v>
       </c>
@@ -8371,7 +9377,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="85">
+    <row r="2" spans="1:4" ht="45">
       <c r="A2" t="s">
         <v>318</v>
       </c>
@@ -8385,7 +9391,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="51">
+    <row r="3" spans="1:4" ht="30">
       <c r="A3" t="s">
         <v>321</v>
       </c>
@@ -8399,7 +9405,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="51">
+    <row r="4" spans="1:4" ht="30">
       <c r="A4" t="s">
         <v>323</v>
       </c>
@@ -8413,7 +9419,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="85">
+    <row r="5" spans="1:4" ht="60">
       <c r="A5" t="s">
         <v>325</v>
       </c>
@@ -8424,7 +9430,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="51">
+    <row r="6" spans="1:4" ht="30">
       <c r="A6" t="s">
         <v>327</v>
       </c>
@@ -8435,7 +9441,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="51">
+    <row r="7" spans="1:4" ht="30">
       <c r="A7" t="s">
         <v>329</v>
       </c>
@@ -8449,7 +9455,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="136">
+    <row r="8" spans="1:4" ht="75">
       <c r="A8" t="s">
         <v>331</v>
       </c>
@@ -8463,7 +9469,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="85">
+    <row r="9" spans="1:4" ht="60">
       <c r="A9" t="s">
         <v>361</v>
       </c>
@@ -8474,7 +9480,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="85">
+    <row r="10" spans="1:4" ht="45">
       <c r="A10" t="s">
         <v>385</v>
       </c>
@@ -8485,7 +9491,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="102">
+    <row r="11" spans="1:4" ht="60">
       <c r="A11" t="s">
         <v>339</v>
       </c>
@@ -8496,7 +9502,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="68">
+    <row r="12" spans="1:4" ht="45">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -8507,7 +9513,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="119">
+    <row r="13" spans="1:4" ht="75">
       <c r="A13" t="s">
         <v>379</v>
       </c>
@@ -8518,7 +9524,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="170">
+    <row r="14" spans="1:4" ht="105">
       <c r="A14" t="s">
         <v>363</v>
       </c>
@@ -8529,7 +9535,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="68">
+    <row r="15" spans="1:4" ht="45">
       <c r="A15" t="s">
         <v>341</v>
       </c>
@@ -8540,7 +9546,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="51">
+    <row r="16" spans="1:4" ht="30">
       <c r="A16" t="s">
         <v>343</v>
       </c>
@@ -8551,7 +9557,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="51">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>333</v>
       </c>
@@ -8562,7 +9568,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="51">
+    <row r="18" spans="1:3" ht="30">
       <c r="A18" t="s">
         <v>371</v>
       </c>
@@ -8573,7 +9579,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="34">
+    <row r="19" spans="1:3" ht="30">
       <c r="A19" t="s">
         <v>345</v>
       </c>
@@ -8584,7 +9590,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="51">
+    <row r="20" spans="1:3" ht="30">
       <c r="A20" t="s">
         <v>347</v>
       </c>
@@ -8595,7 +9601,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="68">
+    <row r="21" spans="1:3" ht="45">
       <c r="A21" t="s">
         <v>359</v>
       </c>
@@ -8606,7 +9612,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="68">
+    <row r="22" spans="1:3" ht="45">
       <c r="A22" t="s">
         <v>349</v>
       </c>
@@ -8617,7 +9623,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="68">
+    <row r="23" spans="1:3" ht="45">
       <c r="A23" t="s">
         <v>351</v>
       </c>
@@ -8628,7 +9634,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="85">
+    <row r="24" spans="1:3" ht="60">
       <c r="A24" t="s">
         <v>365</v>
       </c>
@@ -8639,7 +9645,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="119">
+    <row r="25" spans="1:3" ht="75">
       <c r="A25" t="s">
         <v>367</v>
       </c>
@@ -8650,7 +9656,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="85">
+    <row r="26" spans="1:3" ht="45">
       <c r="A26" t="s">
         <v>369</v>
       </c>
@@ -8661,7 +9667,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="356">
+    <row r="27" spans="1:3" ht="195">
       <c r="A27" t="s">
         <v>353</v>
       </c>
@@ -8672,7 +9678,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="51">
+    <row r="28" spans="1:3" ht="30">
       <c r="A28" t="s">
         <v>373</v>
       </c>
@@ -8683,7 +9689,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="68">
+    <row r="29" spans="1:3" ht="45">
       <c r="A29" t="s">
         <v>375</v>
       </c>
@@ -8694,7 +9700,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="51">
+    <row r="30" spans="1:3" ht="30">
       <c r="A30" t="s">
         <v>335</v>
       </c>
@@ -8705,7 +9711,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="51">
+    <row r="31" spans="1:3" ht="30">
       <c r="A31" t="s">
         <v>377</v>
       </c>
@@ -8716,7 +9722,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="68">
+    <row r="32" spans="1:3" ht="45">
       <c r="A32" t="s">
         <v>355</v>
       </c>
@@ -8727,7 +9733,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="51">
+    <row r="33" spans="1:4" ht="30">
       <c r="A33" t="s">
         <v>337</v>
       </c>
@@ -8741,7 +9747,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="85">
+    <row r="34" spans="1:4" ht="60">
       <c r="A34" t="s">
         <v>381</v>
       </c>
@@ -8752,7 +9758,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="102">
+    <row r="35" spans="1:4" ht="60">
       <c r="A35" t="s">
         <v>383</v>
       </c>
@@ -8763,7 +9769,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="68">
+    <row r="36" spans="1:4" ht="45">
       <c r="A36" t="s">
         <v>357</v>
       </c>
@@ -8774,7 +9780,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="68">
+    <row r="37" spans="1:4" ht="45">
       <c r="A37" t="s">
         <v>387</v>
       </c>
@@ -8785,7 +9791,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="85">
+    <row r="38" spans="1:4" ht="60">
       <c r="A38" t="s">
         <v>389</v>
       </c>
@@ -8796,7 +9802,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="85">
+    <row r="39" spans="1:4" ht="45">
       <c r="A39" t="s">
         <v>208</v>
       </c>
@@ -8807,7 +9813,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="85">
+    <row r="40" spans="1:4" ht="60">
       <c r="A40" t="s">
         <v>210</v>
       </c>
@@ -8818,7 +9824,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="68">
+    <row r="41" spans="1:4" ht="45">
       <c r="A41" t="s">
         <v>75</v>
       </c>
@@ -8829,7 +9835,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="68">
+    <row r="42" spans="1:4" ht="45">
       <c r="A42" t="s">
         <v>212</v>
       </c>
@@ -8840,7 +9846,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="85">
+    <row r="43" spans="1:4" ht="60">
       <c r="A43" t="s">
         <v>214</v>
       </c>

</xml_diff>